<commit_message>
add tc and edit in readme
</commit_message>
<xml_diff>
--- a/test-cases.xlsx
+++ b/test-cases.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="171">
   <si>
     <t>ID</t>
   </si>
@@ -3329,6 +3329,75 @@
   <si>
     <r>
       <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Предусловия:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Роль пользователя - администратор;
+2. Пользователь находится на дашборде;
+3. Есть доступ к почте клиента;
+4. Есть доступ к личному кабинету клиента;
+5. Есть доступ от почты администратора.
+6. На дашборде есть карточка EDIT_NOT_CONFIRMED.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Шаги воспроизведения:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Найти карточку клиента из предусловий;
+2. Удалить карточку с дашборда;
+3. Проверить, что в таблице БД status_hystory появилась соответствующая запись о присвоении статуса карточке;
+4. Проверить, что в БД т card_client статус карточки DELETED;
+5. Перейти в почту клиента и проверить, что ему отправлено письмо об удалении карточки, в письме нет ссылок, требующих действия со стороны клиента;
+6. Проверить, что администратору на почту не пришло сообщение для клиента.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Ожидаемый результат:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Карточка найдена;
+2. Карточка удалена, не отображается на дашборде;
+3. В таблице БД status_hystory появилась запись о присвоении карточке статуса DELETED;
+4. В БД т card_client статус карточки DELETED;
+5. На почте клиента есть письмо с уведомлением об удалении карочки с дашборда. Письмо носит информативный характери действий со стороны клиента не требует, сслыки нет.
+6. Администратору на почту не пришло сообщение для клиента.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <b/>
       </rPr>
       <t>Дополнительная информация:</t>
@@ -3362,6 +3431,77 @@
   </si>
   <si>
     <t>[Админ][Дашборд] Переход карточки из EDIT_NOT_CONFIRMED-&gt;EDITED</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Предусловия:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Роль пользователя - администратор;
+2. Пользователь находится на дашборде;
+3. Есть доступ к почте клиента;
+4. Есть доступ к личному кабинету клиента;
+5. Есть доступ от почты администратора.
+6. На дашборде есть карточка EDIT_NOT_CONFIRMED.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Шаги воспроизведения:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Найти карточку клиента из предусловий;
+2. Изменить данные карточки;
+3. Проверить, что статус карточки изменился на EDITED;
+4. Проверить, что в таблице БД status_hystory появилась соответствующая запись о присвоении статуса карточке;
+5. Проверить, что в БД т card_client статус карточки EDITED;
+6. Проверить, что клиенту отправлено со ссылкой на подтверждение изменений данных в карточке;
+7. Проверить, что администратору не отправлено письмо клиенту.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+      </rPr>
+      <t>Ожидаемый результат:</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">
+1. Карточка найдена;
+2. Данные карточки изменены, изменения сохранены;
+3. Статус карточки на дашборде изменился на EDITED;
+4. В таблице БД status_hystory появилась запись о присвоении карточке статуса EDITED;
+5. В БД т card_client статус карточки EDITED;
+6. Клиенту отправлено со ссылкой на подтверждение изменений данных в карточке;
+7. Администратору не отправлено письмо клиенту.</t>
+    </r>
   </si>
   <si>
     <r>
@@ -3487,7 +3627,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3562,12 +3702,6 @@
     </xf>
     <xf borderId="1" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
@@ -12547,11 +12681,17 @@
       <c r="B10" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
+      <c r="C10" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>164</v>
+      </c>
       <c r="F10" s="20" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11">
@@ -12559,3081 +12699,3087 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
+        <v>166</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>169</v>
+      </c>
       <c r="F11" s="21" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="27"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
     </row>
     <row r="13">
-      <c r="A13" s="27"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
     </row>
     <row r="14">
-      <c r="A14" s="27"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
     </row>
     <row r="15">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
     </row>
     <row r="16">
-      <c r="A16" s="27"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
     </row>
     <row r="17">
-      <c r="A17" s="27"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
     </row>
     <row r="18">
-      <c r="A18" s="27"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
     </row>
     <row r="19">
-      <c r="A19" s="27"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
     </row>
     <row r="20">
-      <c r="A20" s="27"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
     </row>
     <row r="21">
-      <c r="A21" s="27"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
     </row>
     <row r="22">
-      <c r="A22" s="27"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
     </row>
     <row r="23">
-      <c r="A23" s="27"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
     </row>
     <row r="24">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
     </row>
     <row r="25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
     </row>
     <row r="26">
-      <c r="A26" s="27"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
     </row>
     <row r="27">
-      <c r="A27" s="27"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
     </row>
     <row r="28">
-      <c r="A28" s="27"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
     </row>
     <row r="29">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
     </row>
     <row r="30">
-      <c r="A30" s="27"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
     </row>
     <row r="31">
-      <c r="A31" s="27"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28"/>
     </row>
     <row r="32">
-      <c r="A32" s="27"/>
+      <c r="A32" s="25"/>
     </row>
     <row r="33">
-      <c r="A33" s="27"/>
+      <c r="A33" s="25"/>
     </row>
     <row r="34">
-      <c r="A34" s="27"/>
+      <c r="A34" s="25"/>
     </row>
     <row r="35">
-      <c r="A35" s="27"/>
+      <c r="A35" s="25"/>
     </row>
     <row r="36">
-      <c r="A36" s="27"/>
+      <c r="A36" s="25"/>
     </row>
     <row r="37">
-      <c r="A37" s="27"/>
+      <c r="A37" s="25"/>
     </row>
     <row r="38">
-      <c r="A38" s="27"/>
+      <c r="A38" s="25"/>
     </row>
     <row r="39">
-      <c r="A39" s="27"/>
+      <c r="A39" s="25"/>
     </row>
     <row r="40">
-      <c r="A40" s="27"/>
+      <c r="A40" s="25"/>
     </row>
     <row r="41">
-      <c r="A41" s="27"/>
+      <c r="A41" s="25"/>
     </row>
     <row r="42">
-      <c r="A42" s="27"/>
+      <c r="A42" s="25"/>
     </row>
     <row r="43">
-      <c r="A43" s="27"/>
+      <c r="A43" s="25"/>
     </row>
     <row r="44">
-      <c r="A44" s="27"/>
+      <c r="A44" s="25"/>
     </row>
     <row r="45">
-      <c r="A45" s="27"/>
+      <c r="A45" s="25"/>
     </row>
     <row r="46">
-      <c r="A46" s="27"/>
+      <c r="A46" s="25"/>
     </row>
     <row r="47">
-      <c r="A47" s="27"/>
+      <c r="A47" s="25"/>
     </row>
     <row r="48">
-      <c r="A48" s="27"/>
+      <c r="A48" s="25"/>
     </row>
     <row r="49">
-      <c r="A49" s="27"/>
+      <c r="A49" s="25"/>
     </row>
     <row r="50">
-      <c r="A50" s="27"/>
+      <c r="A50" s="25"/>
     </row>
     <row r="51">
-      <c r="A51" s="27"/>
+      <c r="A51" s="25"/>
     </row>
     <row r="52">
-      <c r="A52" s="27"/>
+      <c r="A52" s="25"/>
     </row>
     <row r="53">
-      <c r="A53" s="27"/>
+      <c r="A53" s="25"/>
     </row>
     <row r="54">
-      <c r="A54" s="27"/>
+      <c r="A54" s="25"/>
     </row>
     <row r="55">
-      <c r="A55" s="27"/>
+      <c r="A55" s="25"/>
     </row>
     <row r="56">
-      <c r="A56" s="27"/>
+      <c r="A56" s="25"/>
     </row>
     <row r="57">
-      <c r="A57" s="27"/>
+      <c r="A57" s="25"/>
     </row>
     <row r="58">
-      <c r="A58" s="27"/>
+      <c r="A58" s="25"/>
     </row>
     <row r="59">
-      <c r="A59" s="27"/>
+      <c r="A59" s="25"/>
     </row>
     <row r="60">
-      <c r="A60" s="27"/>
+      <c r="A60" s="25"/>
     </row>
     <row r="61">
-      <c r="A61" s="27"/>
+      <c r="A61" s="25"/>
     </row>
     <row r="62">
-      <c r="A62" s="27"/>
+      <c r="A62" s="25"/>
     </row>
     <row r="63">
-      <c r="A63" s="27"/>
+      <c r="A63" s="25"/>
     </row>
     <row r="64">
-      <c r="A64" s="27"/>
+      <c r="A64" s="25"/>
     </row>
     <row r="65">
-      <c r="A65" s="27"/>
+      <c r="A65" s="25"/>
     </row>
     <row r="66">
-      <c r="A66" s="27"/>
+      <c r="A66" s="25"/>
     </row>
     <row r="67">
-      <c r="A67" s="27"/>
+      <c r="A67" s="25"/>
     </row>
     <row r="68">
-      <c r="A68" s="27"/>
+      <c r="A68" s="25"/>
     </row>
     <row r="69">
-      <c r="A69" s="27"/>
+      <c r="A69" s="25"/>
     </row>
     <row r="70">
-      <c r="A70" s="27"/>
+      <c r="A70" s="25"/>
     </row>
     <row r="71">
-      <c r="A71" s="27"/>
+      <c r="A71" s="25"/>
     </row>
     <row r="72">
-      <c r="A72" s="27"/>
+      <c r="A72" s="25"/>
     </row>
     <row r="73">
-      <c r="A73" s="27"/>
+      <c r="A73" s="25"/>
     </row>
     <row r="74">
-      <c r="A74" s="27"/>
+      <c r="A74" s="25"/>
     </row>
     <row r="75">
-      <c r="A75" s="27"/>
+      <c r="A75" s="25"/>
     </row>
     <row r="76">
-      <c r="A76" s="27"/>
+      <c r="A76" s="25"/>
     </row>
     <row r="77">
-      <c r="A77" s="27"/>
+      <c r="A77" s="25"/>
     </row>
     <row r="78">
-      <c r="A78" s="27"/>
+      <c r="A78" s="25"/>
     </row>
     <row r="79">
-      <c r="A79" s="27"/>
+      <c r="A79" s="25"/>
     </row>
     <row r="80">
-      <c r="A80" s="27"/>
+      <c r="A80" s="25"/>
     </row>
     <row r="81">
-      <c r="A81" s="27"/>
+      <c r="A81" s="25"/>
     </row>
     <row r="82">
-      <c r="A82" s="27"/>
+      <c r="A82" s="25"/>
     </row>
     <row r="83">
-      <c r="A83" s="27"/>
+      <c r="A83" s="25"/>
     </row>
     <row r="84">
-      <c r="A84" s="27"/>
+      <c r="A84" s="25"/>
     </row>
     <row r="85">
-      <c r="A85" s="27"/>
+      <c r="A85" s="25"/>
     </row>
     <row r="86">
-      <c r="A86" s="27"/>
+      <c r="A86" s="25"/>
     </row>
     <row r="87">
-      <c r="A87" s="27"/>
+      <c r="A87" s="25"/>
     </row>
     <row r="88">
-      <c r="A88" s="27"/>
+      <c r="A88" s="25"/>
     </row>
     <row r="89">
-      <c r="A89" s="27"/>
+      <c r="A89" s="25"/>
     </row>
     <row r="90">
-      <c r="A90" s="27"/>
+      <c r="A90" s="25"/>
     </row>
     <row r="91">
-      <c r="A91" s="27"/>
+      <c r="A91" s="25"/>
     </row>
     <row r="92">
-      <c r="A92" s="27"/>
+      <c r="A92" s="25"/>
     </row>
     <row r="93">
-      <c r="A93" s="27"/>
+      <c r="A93" s="25"/>
     </row>
     <row r="94">
-      <c r="A94" s="27"/>
+      <c r="A94" s="25"/>
     </row>
     <row r="95">
-      <c r="A95" s="27"/>
+      <c r="A95" s="25"/>
     </row>
     <row r="96">
-      <c r="A96" s="27"/>
+      <c r="A96" s="25"/>
     </row>
     <row r="97">
-      <c r="A97" s="27"/>
+      <c r="A97" s="25"/>
     </row>
     <row r="98">
-      <c r="A98" s="27"/>
+      <c r="A98" s="25"/>
     </row>
     <row r="99">
-      <c r="A99" s="27"/>
+      <c r="A99" s="25"/>
     </row>
     <row r="100">
-      <c r="A100" s="27"/>
+      <c r="A100" s="25"/>
     </row>
     <row r="101">
-      <c r="A101" s="27"/>
+      <c r="A101" s="25"/>
     </row>
     <row r="102">
-      <c r="A102" s="27"/>
+      <c r="A102" s="25"/>
     </row>
     <row r="103">
-      <c r="A103" s="27"/>
+      <c r="A103" s="25"/>
     </row>
     <row r="104">
-      <c r="A104" s="27"/>
+      <c r="A104" s="25"/>
     </row>
     <row r="105">
-      <c r="A105" s="27"/>
+      <c r="A105" s="25"/>
     </row>
     <row r="106">
-      <c r="A106" s="27"/>
+      <c r="A106" s="25"/>
     </row>
     <row r="107">
-      <c r="A107" s="27"/>
+      <c r="A107" s="25"/>
     </row>
     <row r="108">
-      <c r="A108" s="27"/>
+      <c r="A108" s="25"/>
     </row>
     <row r="109">
-      <c r="A109" s="27"/>
+      <c r="A109" s="25"/>
     </row>
     <row r="110">
-      <c r="A110" s="27"/>
+      <c r="A110" s="25"/>
     </row>
     <row r="111">
-      <c r="A111" s="27"/>
+      <c r="A111" s="25"/>
     </row>
     <row r="112">
-      <c r="A112" s="27"/>
+      <c r="A112" s="25"/>
     </row>
     <row r="113">
-      <c r="A113" s="27"/>
+      <c r="A113" s="25"/>
     </row>
     <row r="114">
-      <c r="A114" s="27"/>
+      <c r="A114" s="25"/>
     </row>
     <row r="115">
-      <c r="A115" s="27"/>
+      <c r="A115" s="25"/>
     </row>
     <row r="116">
-      <c r="A116" s="27"/>
+      <c r="A116" s="25"/>
     </row>
     <row r="117">
-      <c r="A117" s="27"/>
+      <c r="A117" s="25"/>
     </row>
     <row r="118">
-      <c r="A118" s="27"/>
+      <c r="A118" s="25"/>
     </row>
     <row r="119">
-      <c r="A119" s="27"/>
+      <c r="A119" s="25"/>
     </row>
     <row r="120">
-      <c r="A120" s="27"/>
+      <c r="A120" s="25"/>
     </row>
     <row r="121">
-      <c r="A121" s="27"/>
+      <c r="A121" s="25"/>
     </row>
     <row r="122">
-      <c r="A122" s="27"/>
+      <c r="A122" s="25"/>
     </row>
     <row r="123">
-      <c r="A123" s="27"/>
+      <c r="A123" s="25"/>
     </row>
     <row r="124">
-      <c r="A124" s="27"/>
+      <c r="A124" s="25"/>
     </row>
     <row r="125">
-      <c r="A125" s="27"/>
+      <c r="A125" s="25"/>
     </row>
     <row r="126">
-      <c r="A126" s="27"/>
+      <c r="A126" s="25"/>
     </row>
     <row r="127">
-      <c r="A127" s="27"/>
+      <c r="A127" s="25"/>
     </row>
     <row r="128">
-      <c r="A128" s="27"/>
+      <c r="A128" s="25"/>
     </row>
     <row r="129">
-      <c r="A129" s="27"/>
+      <c r="A129" s="25"/>
     </row>
     <row r="130">
-      <c r="A130" s="27"/>
+      <c r="A130" s="25"/>
     </row>
     <row r="131">
-      <c r="A131" s="27"/>
+      <c r="A131" s="25"/>
     </row>
     <row r="132">
-      <c r="A132" s="27"/>
+      <c r="A132" s="25"/>
     </row>
     <row r="133">
-      <c r="A133" s="27"/>
+      <c r="A133" s="25"/>
     </row>
     <row r="134">
-      <c r="A134" s="27"/>
+      <c r="A134" s="25"/>
     </row>
     <row r="135">
-      <c r="A135" s="27"/>
+      <c r="A135" s="25"/>
     </row>
     <row r="136">
-      <c r="A136" s="27"/>
+      <c r="A136" s="25"/>
     </row>
     <row r="137">
-      <c r="A137" s="27"/>
+      <c r="A137" s="25"/>
     </row>
     <row r="138">
-      <c r="A138" s="27"/>
+      <c r="A138" s="25"/>
     </row>
     <row r="139">
-      <c r="A139" s="27"/>
+      <c r="A139" s="25"/>
     </row>
     <row r="140">
-      <c r="A140" s="27"/>
+      <c r="A140" s="25"/>
     </row>
     <row r="141">
-      <c r="A141" s="27"/>
+      <c r="A141" s="25"/>
     </row>
     <row r="142">
-      <c r="A142" s="27"/>
+      <c r="A142" s="25"/>
     </row>
     <row r="143">
-      <c r="A143" s="27"/>
+      <c r="A143" s="25"/>
     </row>
     <row r="144">
-      <c r="A144" s="27"/>
+      <c r="A144" s="25"/>
     </row>
     <row r="145">
-      <c r="A145" s="27"/>
+      <c r="A145" s="25"/>
     </row>
     <row r="146">
-      <c r="A146" s="27"/>
+      <c r="A146" s="25"/>
     </row>
     <row r="147">
-      <c r="A147" s="27"/>
+      <c r="A147" s="25"/>
     </row>
     <row r="148">
-      <c r="A148" s="27"/>
+      <c r="A148" s="25"/>
     </row>
     <row r="149">
-      <c r="A149" s="27"/>
+      <c r="A149" s="25"/>
     </row>
     <row r="150">
-      <c r="A150" s="27"/>
+      <c r="A150" s="25"/>
     </row>
     <row r="151">
-      <c r="A151" s="27"/>
+      <c r="A151" s="25"/>
     </row>
     <row r="152">
-      <c r="A152" s="27"/>
+      <c r="A152" s="25"/>
     </row>
     <row r="153">
-      <c r="A153" s="27"/>
+      <c r="A153" s="25"/>
     </row>
     <row r="154">
-      <c r="A154" s="27"/>
+      <c r="A154" s="25"/>
     </row>
     <row r="155">
-      <c r="A155" s="27"/>
+      <c r="A155" s="25"/>
     </row>
     <row r="156">
-      <c r="A156" s="27"/>
+      <c r="A156" s="25"/>
     </row>
     <row r="157">
-      <c r="A157" s="27"/>
+      <c r="A157" s="25"/>
     </row>
     <row r="158">
-      <c r="A158" s="27"/>
+      <c r="A158" s="25"/>
     </row>
     <row r="159">
-      <c r="A159" s="27"/>
+      <c r="A159" s="25"/>
     </row>
     <row r="160">
-      <c r="A160" s="27"/>
+      <c r="A160" s="25"/>
     </row>
     <row r="161">
-      <c r="A161" s="27"/>
+      <c r="A161" s="25"/>
     </row>
     <row r="162">
-      <c r="A162" s="27"/>
+      <c r="A162" s="25"/>
     </row>
     <row r="163">
-      <c r="A163" s="27"/>
+      <c r="A163" s="25"/>
     </row>
     <row r="164">
-      <c r="A164" s="27"/>
+      <c r="A164" s="25"/>
     </row>
     <row r="165">
-      <c r="A165" s="27"/>
+      <c r="A165" s="25"/>
     </row>
     <row r="166">
-      <c r="A166" s="27"/>
+      <c r="A166" s="25"/>
     </row>
     <row r="167">
-      <c r="A167" s="27"/>
+      <c r="A167" s="25"/>
     </row>
     <row r="168">
-      <c r="A168" s="27"/>
+      <c r="A168" s="25"/>
     </row>
     <row r="169">
-      <c r="A169" s="27"/>
+      <c r="A169" s="25"/>
     </row>
     <row r="170">
-      <c r="A170" s="27"/>
+      <c r="A170" s="25"/>
     </row>
     <row r="171">
-      <c r="A171" s="27"/>
+      <c r="A171" s="25"/>
     </row>
     <row r="172">
-      <c r="A172" s="27"/>
+      <c r="A172" s="25"/>
     </row>
     <row r="173">
-      <c r="A173" s="27"/>
+      <c r="A173" s="25"/>
     </row>
     <row r="174">
-      <c r="A174" s="27"/>
+      <c r="A174" s="25"/>
     </row>
     <row r="175">
-      <c r="A175" s="27"/>
+      <c r="A175" s="25"/>
     </row>
     <row r="176">
-      <c r="A176" s="27"/>
+      <c r="A176" s="25"/>
     </row>
     <row r="177">
-      <c r="A177" s="27"/>
+      <c r="A177" s="25"/>
     </row>
     <row r="178">
-      <c r="A178" s="27"/>
+      <c r="A178" s="25"/>
     </row>
     <row r="179">
-      <c r="A179" s="27"/>
+      <c r="A179" s="25"/>
     </row>
     <row r="180">
-      <c r="A180" s="27"/>
+      <c r="A180" s="25"/>
     </row>
     <row r="181">
-      <c r="A181" s="27"/>
+      <c r="A181" s="25"/>
     </row>
     <row r="182">
-      <c r="A182" s="27"/>
+      <c r="A182" s="25"/>
     </row>
     <row r="183">
-      <c r="A183" s="27"/>
+      <c r="A183" s="25"/>
     </row>
     <row r="184">
-      <c r="A184" s="27"/>
+      <c r="A184" s="25"/>
     </row>
     <row r="185">
-      <c r="A185" s="27"/>
+      <c r="A185" s="25"/>
     </row>
     <row r="186">
-      <c r="A186" s="27"/>
+      <c r="A186" s="25"/>
     </row>
     <row r="187">
-      <c r="A187" s="27"/>
+      <c r="A187" s="25"/>
     </row>
     <row r="188">
-      <c r="A188" s="27"/>
+      <c r="A188" s="25"/>
     </row>
     <row r="189">
-      <c r="A189" s="27"/>
+      <c r="A189" s="25"/>
     </row>
     <row r="190">
-      <c r="A190" s="27"/>
+      <c r="A190" s="25"/>
     </row>
     <row r="191">
-      <c r="A191" s="27"/>
+      <c r="A191" s="25"/>
     </row>
     <row r="192">
-      <c r="A192" s="27"/>
+      <c r="A192" s="25"/>
     </row>
     <row r="193">
-      <c r="A193" s="27"/>
+      <c r="A193" s="25"/>
     </row>
     <row r="194">
-      <c r="A194" s="27"/>
+      <c r="A194" s="25"/>
     </row>
     <row r="195">
-      <c r="A195" s="27"/>
+      <c r="A195" s="25"/>
     </row>
     <row r="196">
-      <c r="A196" s="27"/>
+      <c r="A196" s="25"/>
     </row>
     <row r="197">
-      <c r="A197" s="27"/>
+      <c r="A197" s="25"/>
     </row>
     <row r="198">
-      <c r="A198" s="27"/>
+      <c r="A198" s="25"/>
     </row>
     <row r="199">
-      <c r="A199" s="27"/>
+      <c r="A199" s="25"/>
     </row>
     <row r="200">
-      <c r="A200" s="27"/>
+      <c r="A200" s="25"/>
     </row>
     <row r="201">
-      <c r="A201" s="27"/>
+      <c r="A201" s="25"/>
     </row>
     <row r="202">
-      <c r="A202" s="27"/>
+      <c r="A202" s="25"/>
     </row>
     <row r="203">
-      <c r="A203" s="27"/>
+      <c r="A203" s="25"/>
     </row>
     <row r="204">
-      <c r="A204" s="27"/>
+      <c r="A204" s="25"/>
     </row>
     <row r="205">
-      <c r="A205" s="27"/>
+      <c r="A205" s="25"/>
     </row>
     <row r="206">
-      <c r="A206" s="27"/>
+      <c r="A206" s="25"/>
     </row>
     <row r="207">
-      <c r="A207" s="27"/>
+      <c r="A207" s="25"/>
     </row>
     <row r="208">
-      <c r="A208" s="27"/>
+      <c r="A208" s="25"/>
     </row>
     <row r="209">
-      <c r="A209" s="27"/>
+      <c r="A209" s="25"/>
     </row>
     <row r="210">
-      <c r="A210" s="27"/>
+      <c r="A210" s="25"/>
     </row>
     <row r="211">
-      <c r="A211" s="27"/>
+      <c r="A211" s="25"/>
     </row>
     <row r="212">
-      <c r="A212" s="27"/>
+      <c r="A212" s="25"/>
     </row>
     <row r="213">
-      <c r="A213" s="27"/>
+      <c r="A213" s="25"/>
     </row>
     <row r="214">
-      <c r="A214" s="27"/>
+      <c r="A214" s="25"/>
     </row>
     <row r="215">
-      <c r="A215" s="27"/>
+      <c r="A215" s="25"/>
     </row>
     <row r="216">
-      <c r="A216" s="27"/>
+      <c r="A216" s="25"/>
     </row>
     <row r="217">
-      <c r="A217" s="27"/>
+      <c r="A217" s="25"/>
     </row>
     <row r="218">
-      <c r="A218" s="27"/>
+      <c r="A218" s="25"/>
     </row>
     <row r="219">
-      <c r="A219" s="27"/>
+      <c r="A219" s="25"/>
     </row>
     <row r="220">
-      <c r="A220" s="27"/>
+      <c r="A220" s="25"/>
     </row>
     <row r="221">
-      <c r="A221" s="27"/>
+      <c r="A221" s="25"/>
     </row>
     <row r="222">
-      <c r="A222" s="27"/>
+      <c r="A222" s="25"/>
     </row>
     <row r="223">
-      <c r="A223" s="27"/>
+      <c r="A223" s="25"/>
     </row>
     <row r="224">
-      <c r="A224" s="27"/>
+      <c r="A224" s="25"/>
     </row>
     <row r="225">
-      <c r="A225" s="27"/>
+      <c r="A225" s="25"/>
     </row>
     <row r="226">
-      <c r="A226" s="27"/>
+      <c r="A226" s="25"/>
     </row>
     <row r="227">
-      <c r="A227" s="27"/>
+      <c r="A227" s="25"/>
     </row>
     <row r="228">
-      <c r="A228" s="27"/>
+      <c r="A228" s="25"/>
     </row>
     <row r="229">
-      <c r="A229" s="27"/>
+      <c r="A229" s="25"/>
     </row>
     <row r="230">
-      <c r="A230" s="27"/>
+      <c r="A230" s="25"/>
     </row>
     <row r="231">
-      <c r="A231" s="27"/>
+      <c r="A231" s="25"/>
     </row>
     <row r="232">
-      <c r="A232" s="27"/>
+      <c r="A232" s="25"/>
     </row>
     <row r="233">
-      <c r="A233" s="27"/>
+      <c r="A233" s="25"/>
     </row>
     <row r="234">
-      <c r="A234" s="27"/>
+      <c r="A234" s="25"/>
     </row>
     <row r="235">
-      <c r="A235" s="27"/>
+      <c r="A235" s="25"/>
     </row>
     <row r="236">
-      <c r="A236" s="27"/>
+      <c r="A236" s="25"/>
     </row>
     <row r="237">
-      <c r="A237" s="27"/>
+      <c r="A237" s="25"/>
     </row>
     <row r="238">
-      <c r="A238" s="27"/>
+      <c r="A238" s="25"/>
     </row>
     <row r="239">
-      <c r="A239" s="27"/>
+      <c r="A239" s="25"/>
     </row>
     <row r="240">
-      <c r="A240" s="27"/>
+      <c r="A240" s="25"/>
     </row>
     <row r="241">
-      <c r="A241" s="27"/>
+      <c r="A241" s="25"/>
     </row>
     <row r="242">
-      <c r="A242" s="27"/>
+      <c r="A242" s="25"/>
     </row>
     <row r="243">
-      <c r="A243" s="27"/>
+      <c r="A243" s="25"/>
     </row>
     <row r="244">
-      <c r="A244" s="27"/>
+      <c r="A244" s="25"/>
     </row>
     <row r="245">
-      <c r="A245" s="27"/>
+      <c r="A245" s="25"/>
     </row>
     <row r="246">
-      <c r="A246" s="27"/>
+      <c r="A246" s="25"/>
     </row>
     <row r="247">
-      <c r="A247" s="27"/>
+      <c r="A247" s="25"/>
     </row>
     <row r="248">
-      <c r="A248" s="27"/>
+      <c r="A248" s="25"/>
     </row>
     <row r="249">
-      <c r="A249" s="27"/>
+      <c r="A249" s="25"/>
     </row>
     <row r="250">
-      <c r="A250" s="27"/>
+      <c r="A250" s="25"/>
     </row>
     <row r="251">
-      <c r="A251" s="27"/>
+      <c r="A251" s="25"/>
     </row>
     <row r="252">
-      <c r="A252" s="27"/>
+      <c r="A252" s="25"/>
     </row>
     <row r="253">
-      <c r="A253" s="27"/>
+      <c r="A253" s="25"/>
     </row>
     <row r="254">
-      <c r="A254" s="27"/>
+      <c r="A254" s="25"/>
     </row>
     <row r="255">
-      <c r="A255" s="27"/>
+      <c r="A255" s="25"/>
     </row>
     <row r="256">
-      <c r="A256" s="27"/>
+      <c r="A256" s="25"/>
     </row>
     <row r="257">
-      <c r="A257" s="27"/>
+      <c r="A257" s="25"/>
     </row>
     <row r="258">
-      <c r="A258" s="27"/>
+      <c r="A258" s="25"/>
     </row>
     <row r="259">
-      <c r="A259" s="27"/>
+      <c r="A259" s="25"/>
     </row>
     <row r="260">
-      <c r="A260" s="27"/>
+      <c r="A260" s="25"/>
     </row>
     <row r="261">
-      <c r="A261" s="27"/>
+      <c r="A261" s="25"/>
     </row>
     <row r="262">
-      <c r="A262" s="27"/>
+      <c r="A262" s="25"/>
     </row>
     <row r="263">
-      <c r="A263" s="27"/>
+      <c r="A263" s="25"/>
     </row>
     <row r="264">
-      <c r="A264" s="27"/>
+      <c r="A264" s="25"/>
     </row>
     <row r="265">
-      <c r="A265" s="27"/>
+      <c r="A265" s="25"/>
     </row>
     <row r="266">
-      <c r="A266" s="27"/>
+      <c r="A266" s="25"/>
     </row>
     <row r="267">
-      <c r="A267" s="27"/>
+      <c r="A267" s="25"/>
     </row>
     <row r="268">
-      <c r="A268" s="27"/>
+      <c r="A268" s="25"/>
     </row>
     <row r="269">
-      <c r="A269" s="27"/>
+      <c r="A269" s="25"/>
     </row>
     <row r="270">
-      <c r="A270" s="27"/>
+      <c r="A270" s="25"/>
     </row>
     <row r="271">
-      <c r="A271" s="27"/>
+      <c r="A271" s="25"/>
     </row>
     <row r="272">
-      <c r="A272" s="27"/>
+      <c r="A272" s="25"/>
     </row>
     <row r="273">
-      <c r="A273" s="27"/>
+      <c r="A273" s="25"/>
     </row>
     <row r="274">
-      <c r="A274" s="27"/>
+      <c r="A274" s="25"/>
     </row>
     <row r="275">
-      <c r="A275" s="27"/>
+      <c r="A275" s="25"/>
     </row>
     <row r="276">
-      <c r="A276" s="27"/>
+      <c r="A276" s="25"/>
     </row>
     <row r="277">
-      <c r="A277" s="27"/>
+      <c r="A277" s="25"/>
     </row>
     <row r="278">
-      <c r="A278" s="27"/>
+      <c r="A278" s="25"/>
     </row>
     <row r="279">
-      <c r="A279" s="27"/>
+      <c r="A279" s="25"/>
     </row>
     <row r="280">
-      <c r="A280" s="27"/>
+      <c r="A280" s="25"/>
     </row>
     <row r="281">
-      <c r="A281" s="27"/>
+      <c r="A281" s="25"/>
     </row>
     <row r="282">
-      <c r="A282" s="27"/>
+      <c r="A282" s="25"/>
     </row>
     <row r="283">
-      <c r="A283" s="27"/>
+      <c r="A283" s="25"/>
     </row>
     <row r="284">
-      <c r="A284" s="27"/>
+      <c r="A284" s="25"/>
     </row>
     <row r="285">
-      <c r="A285" s="27"/>
+      <c r="A285" s="25"/>
     </row>
     <row r="286">
-      <c r="A286" s="27"/>
+      <c r="A286" s="25"/>
     </row>
     <row r="287">
-      <c r="A287" s="27"/>
+      <c r="A287" s="25"/>
     </row>
     <row r="288">
-      <c r="A288" s="27"/>
+      <c r="A288" s="25"/>
     </row>
     <row r="289">
-      <c r="A289" s="27"/>
+      <c r="A289" s="25"/>
     </row>
     <row r="290">
-      <c r="A290" s="27"/>
+      <c r="A290" s="25"/>
     </row>
     <row r="291">
-      <c r="A291" s="27"/>
+      <c r="A291" s="25"/>
     </row>
     <row r="292">
-      <c r="A292" s="27"/>
+      <c r="A292" s="25"/>
     </row>
     <row r="293">
-      <c r="A293" s="27"/>
+      <c r="A293" s="25"/>
     </row>
     <row r="294">
-      <c r="A294" s="27"/>
+      <c r="A294" s="25"/>
     </row>
     <row r="295">
-      <c r="A295" s="27"/>
+      <c r="A295" s="25"/>
     </row>
     <row r="296">
-      <c r="A296" s="27"/>
+      <c r="A296" s="25"/>
     </row>
     <row r="297">
-      <c r="A297" s="27"/>
+      <c r="A297" s="25"/>
     </row>
     <row r="298">
-      <c r="A298" s="27"/>
+      <c r="A298" s="25"/>
     </row>
     <row r="299">
-      <c r="A299" s="27"/>
+      <c r="A299" s="25"/>
     </row>
     <row r="300">
-      <c r="A300" s="27"/>
+      <c r="A300" s="25"/>
     </row>
     <row r="301">
-      <c r="A301" s="27"/>
+      <c r="A301" s="25"/>
     </row>
     <row r="302">
-      <c r="A302" s="27"/>
+      <c r="A302" s="25"/>
     </row>
     <row r="303">
-      <c r="A303" s="27"/>
+      <c r="A303" s="25"/>
     </row>
     <row r="304">
-      <c r="A304" s="27"/>
+      <c r="A304" s="25"/>
     </row>
     <row r="305">
-      <c r="A305" s="27"/>
+      <c r="A305" s="25"/>
     </row>
     <row r="306">
-      <c r="A306" s="27"/>
+      <c r="A306" s="25"/>
     </row>
     <row r="307">
-      <c r="A307" s="27"/>
+      <c r="A307" s="25"/>
     </row>
     <row r="308">
-      <c r="A308" s="27"/>
+      <c r="A308" s="25"/>
     </row>
     <row r="309">
-      <c r="A309" s="27"/>
+      <c r="A309" s="25"/>
     </row>
     <row r="310">
-      <c r="A310" s="27"/>
+      <c r="A310" s="25"/>
     </row>
     <row r="311">
-      <c r="A311" s="27"/>
+      <c r="A311" s="25"/>
     </row>
     <row r="312">
-      <c r="A312" s="27"/>
+      <c r="A312" s="25"/>
     </row>
     <row r="313">
-      <c r="A313" s="27"/>
+      <c r="A313" s="25"/>
     </row>
     <row r="314">
-      <c r="A314" s="27"/>
+      <c r="A314" s="25"/>
     </row>
     <row r="315">
-      <c r="A315" s="27"/>
+      <c r="A315" s="25"/>
     </row>
     <row r="316">
-      <c r="A316" s="27"/>
+      <c r="A316" s="25"/>
     </row>
     <row r="317">
-      <c r="A317" s="27"/>
+      <c r="A317" s="25"/>
     </row>
     <row r="318">
-      <c r="A318" s="27"/>
+      <c r="A318" s="25"/>
     </row>
     <row r="319">
-      <c r="A319" s="27"/>
+      <c r="A319" s="25"/>
     </row>
     <row r="320">
-      <c r="A320" s="27"/>
+      <c r="A320" s="25"/>
     </row>
     <row r="321">
-      <c r="A321" s="27"/>
+      <c r="A321" s="25"/>
     </row>
     <row r="322">
-      <c r="A322" s="27"/>
+      <c r="A322" s="25"/>
     </row>
     <row r="323">
-      <c r="A323" s="27"/>
+      <c r="A323" s="25"/>
     </row>
     <row r="324">
-      <c r="A324" s="27"/>
+      <c r="A324" s="25"/>
     </row>
     <row r="325">
-      <c r="A325" s="27"/>
+      <c r="A325" s="25"/>
     </row>
     <row r="326">
-      <c r="A326" s="27"/>
+      <c r="A326" s="25"/>
     </row>
     <row r="327">
-      <c r="A327" s="27"/>
+      <c r="A327" s="25"/>
     </row>
     <row r="328">
-      <c r="A328" s="27"/>
+      <c r="A328" s="25"/>
     </row>
     <row r="329">
-      <c r="A329" s="27"/>
+      <c r="A329" s="25"/>
     </row>
     <row r="330">
-      <c r="A330" s="27"/>
+      <c r="A330" s="25"/>
     </row>
     <row r="331">
-      <c r="A331" s="27"/>
+      <c r="A331" s="25"/>
     </row>
     <row r="332">
-      <c r="A332" s="27"/>
+      <c r="A332" s="25"/>
     </row>
     <row r="333">
-      <c r="A333" s="27"/>
+      <c r="A333" s="25"/>
     </row>
     <row r="334">
-      <c r="A334" s="27"/>
+      <c r="A334" s="25"/>
     </row>
     <row r="335">
-      <c r="A335" s="27"/>
+      <c r="A335" s="25"/>
     </row>
     <row r="336">
-      <c r="A336" s="27"/>
+      <c r="A336" s="25"/>
     </row>
     <row r="337">
-      <c r="A337" s="27"/>
+      <c r="A337" s="25"/>
     </row>
     <row r="338">
-      <c r="A338" s="27"/>
+      <c r="A338" s="25"/>
     </row>
     <row r="339">
-      <c r="A339" s="27"/>
+      <c r="A339" s="25"/>
     </row>
     <row r="340">
-      <c r="A340" s="27"/>
+      <c r="A340" s="25"/>
     </row>
     <row r="341">
-      <c r="A341" s="27"/>
+      <c r="A341" s="25"/>
     </row>
     <row r="342">
-      <c r="A342" s="27"/>
+      <c r="A342" s="25"/>
     </row>
     <row r="343">
-      <c r="A343" s="27"/>
+      <c r="A343" s="25"/>
     </row>
     <row r="344">
-      <c r="A344" s="27"/>
+      <c r="A344" s="25"/>
     </row>
     <row r="345">
-      <c r="A345" s="27"/>
+      <c r="A345" s="25"/>
     </row>
     <row r="346">
-      <c r="A346" s="27"/>
+      <c r="A346" s="25"/>
     </row>
     <row r="347">
-      <c r="A347" s="27"/>
+      <c r="A347" s="25"/>
     </row>
     <row r="348">
-      <c r="A348" s="27"/>
+      <c r="A348" s="25"/>
     </row>
     <row r="349">
-      <c r="A349" s="27"/>
+      <c r="A349" s="25"/>
     </row>
     <row r="350">
-      <c r="A350" s="27"/>
+      <c r="A350" s="25"/>
     </row>
     <row r="351">
-      <c r="A351" s="27"/>
+      <c r="A351" s="25"/>
     </row>
     <row r="352">
-      <c r="A352" s="27"/>
+      <c r="A352" s="25"/>
     </row>
     <row r="353">
-      <c r="A353" s="27"/>
+      <c r="A353" s="25"/>
     </row>
     <row r="354">
-      <c r="A354" s="27"/>
+      <c r="A354" s="25"/>
     </row>
     <row r="355">
-      <c r="A355" s="27"/>
+      <c r="A355" s="25"/>
     </row>
     <row r="356">
-      <c r="A356" s="27"/>
+      <c r="A356" s="25"/>
     </row>
     <row r="357">
-      <c r="A357" s="27"/>
+      <c r="A357" s="25"/>
     </row>
     <row r="358">
-      <c r="A358" s="27"/>
+      <c r="A358" s="25"/>
     </row>
     <row r="359">
-      <c r="A359" s="27"/>
+      <c r="A359" s="25"/>
     </row>
     <row r="360">
-      <c r="A360" s="27"/>
+      <c r="A360" s="25"/>
     </row>
     <row r="361">
-      <c r="A361" s="27"/>
+      <c r="A361" s="25"/>
     </row>
     <row r="362">
-      <c r="A362" s="27"/>
+      <c r="A362" s="25"/>
     </row>
     <row r="363">
-      <c r="A363" s="27"/>
+      <c r="A363" s="25"/>
     </row>
     <row r="364">
-      <c r="A364" s="27"/>
+      <c r="A364" s="25"/>
     </row>
     <row r="365">
-      <c r="A365" s="27"/>
+      <c r="A365" s="25"/>
     </row>
     <row r="366">
-      <c r="A366" s="27"/>
+      <c r="A366" s="25"/>
     </row>
     <row r="367">
-      <c r="A367" s="27"/>
+      <c r="A367" s="25"/>
     </row>
     <row r="368">
-      <c r="A368" s="27"/>
+      <c r="A368" s="25"/>
     </row>
     <row r="369">
-      <c r="A369" s="27"/>
+      <c r="A369" s="25"/>
     </row>
     <row r="370">
-      <c r="A370" s="27"/>
+      <c r="A370" s="25"/>
     </row>
     <row r="371">
-      <c r="A371" s="27"/>
+      <c r="A371" s="25"/>
     </row>
     <row r="372">
-      <c r="A372" s="27"/>
+      <c r="A372" s="25"/>
     </row>
     <row r="373">
-      <c r="A373" s="27"/>
+      <c r="A373" s="25"/>
     </row>
     <row r="374">
-      <c r="A374" s="27"/>
+      <c r="A374" s="25"/>
     </row>
     <row r="375">
-      <c r="A375" s="27"/>
+      <c r="A375" s="25"/>
     </row>
     <row r="376">
-      <c r="A376" s="27"/>
+      <c r="A376" s="25"/>
     </row>
     <row r="377">
-      <c r="A377" s="27"/>
+      <c r="A377" s="25"/>
     </row>
     <row r="378">
-      <c r="A378" s="27"/>
+      <c r="A378" s="25"/>
     </row>
     <row r="379">
-      <c r="A379" s="27"/>
+      <c r="A379" s="25"/>
     </row>
     <row r="380">
-      <c r="A380" s="27"/>
+      <c r="A380" s="25"/>
     </row>
     <row r="381">
-      <c r="A381" s="27"/>
+      <c r="A381" s="25"/>
     </row>
     <row r="382">
-      <c r="A382" s="27"/>
+      <c r="A382" s="25"/>
     </row>
     <row r="383">
-      <c r="A383" s="27"/>
+      <c r="A383" s="25"/>
     </row>
     <row r="384">
-      <c r="A384" s="27"/>
+      <c r="A384" s="25"/>
     </row>
     <row r="385">
-      <c r="A385" s="27"/>
+      <c r="A385" s="25"/>
     </row>
     <row r="386">
-      <c r="A386" s="27"/>
+      <c r="A386" s="25"/>
     </row>
     <row r="387">
-      <c r="A387" s="27"/>
+      <c r="A387" s="25"/>
     </row>
     <row r="388">
-      <c r="A388" s="27"/>
+      <c r="A388" s="25"/>
     </row>
     <row r="389">
-      <c r="A389" s="27"/>
+      <c r="A389" s="25"/>
     </row>
     <row r="390">
-      <c r="A390" s="27"/>
+      <c r="A390" s="25"/>
     </row>
     <row r="391">
-      <c r="A391" s="27"/>
+      <c r="A391" s="25"/>
     </row>
     <row r="392">
-      <c r="A392" s="27"/>
+      <c r="A392" s="25"/>
     </row>
     <row r="393">
-      <c r="A393" s="27"/>
+      <c r="A393" s="25"/>
     </row>
     <row r="394">
-      <c r="A394" s="27"/>
+      <c r="A394" s="25"/>
     </row>
     <row r="395">
-      <c r="A395" s="27"/>
+      <c r="A395" s="25"/>
     </row>
     <row r="396">
-      <c r="A396" s="27"/>
+      <c r="A396" s="25"/>
     </row>
     <row r="397">
-      <c r="A397" s="27"/>
+      <c r="A397" s="25"/>
     </row>
     <row r="398">
-      <c r="A398" s="27"/>
+      <c r="A398" s="25"/>
     </row>
     <row r="399">
-      <c r="A399" s="27"/>
+      <c r="A399" s="25"/>
     </row>
     <row r="400">
-      <c r="A400" s="27"/>
+      <c r="A400" s="25"/>
     </row>
     <row r="401">
-      <c r="A401" s="27"/>
+      <c r="A401" s="25"/>
     </row>
     <row r="402">
-      <c r="A402" s="27"/>
+      <c r="A402" s="25"/>
     </row>
     <row r="403">
-      <c r="A403" s="27"/>
+      <c r="A403" s="25"/>
     </row>
     <row r="404">
-      <c r="A404" s="27"/>
+      <c r="A404" s="25"/>
     </row>
     <row r="405">
-      <c r="A405" s="27"/>
+      <c r="A405" s="25"/>
     </row>
     <row r="406">
-      <c r="A406" s="27"/>
+      <c r="A406" s="25"/>
     </row>
     <row r="407">
-      <c r="A407" s="27"/>
+      <c r="A407" s="25"/>
     </row>
     <row r="408">
-      <c r="A408" s="27"/>
+      <c r="A408" s="25"/>
     </row>
     <row r="409">
-      <c r="A409" s="27"/>
+      <c r="A409" s="25"/>
     </row>
     <row r="410">
-      <c r="A410" s="27"/>
+      <c r="A410" s="25"/>
     </row>
     <row r="411">
-      <c r="A411" s="27"/>
+      <c r="A411" s="25"/>
     </row>
     <row r="412">
-      <c r="A412" s="27"/>
+      <c r="A412" s="25"/>
     </row>
     <row r="413">
-      <c r="A413" s="27"/>
+      <c r="A413" s="25"/>
     </row>
     <row r="414">
-      <c r="A414" s="27"/>
+      <c r="A414" s="25"/>
     </row>
     <row r="415">
-      <c r="A415" s="27"/>
+      <c r="A415" s="25"/>
     </row>
     <row r="416">
-      <c r="A416" s="27"/>
+      <c r="A416" s="25"/>
     </row>
     <row r="417">
-      <c r="A417" s="27"/>
+      <c r="A417" s="25"/>
     </row>
     <row r="418">
-      <c r="A418" s="27"/>
+      <c r="A418" s="25"/>
     </row>
     <row r="419">
-      <c r="A419" s="27"/>
+      <c r="A419" s="25"/>
     </row>
     <row r="420">
-      <c r="A420" s="27"/>
+      <c r="A420" s="25"/>
     </row>
     <row r="421">
-      <c r="A421" s="27"/>
+      <c r="A421" s="25"/>
     </row>
     <row r="422">
-      <c r="A422" s="27"/>
+      <c r="A422" s="25"/>
     </row>
     <row r="423">
-      <c r="A423" s="27"/>
+      <c r="A423" s="25"/>
     </row>
     <row r="424">
-      <c r="A424" s="27"/>
+      <c r="A424" s="25"/>
     </row>
     <row r="425">
-      <c r="A425" s="27"/>
+      <c r="A425" s="25"/>
     </row>
     <row r="426">
-      <c r="A426" s="27"/>
+      <c r="A426" s="25"/>
     </row>
     <row r="427">
-      <c r="A427" s="27"/>
+      <c r="A427" s="25"/>
     </row>
     <row r="428">
-      <c r="A428" s="27"/>
+      <c r="A428" s="25"/>
     </row>
     <row r="429">
-      <c r="A429" s="27"/>
+      <c r="A429" s="25"/>
     </row>
     <row r="430">
-      <c r="A430" s="27"/>
+      <c r="A430" s="25"/>
     </row>
     <row r="431">
-      <c r="A431" s="27"/>
+      <c r="A431" s="25"/>
     </row>
     <row r="432">
-      <c r="A432" s="27"/>
+      <c r="A432" s="25"/>
     </row>
     <row r="433">
-      <c r="A433" s="27"/>
+      <c r="A433" s="25"/>
     </row>
     <row r="434">
-      <c r="A434" s="27"/>
+      <c r="A434" s="25"/>
     </row>
     <row r="435">
-      <c r="A435" s="27"/>
+      <c r="A435" s="25"/>
     </row>
     <row r="436">
-      <c r="A436" s="27"/>
+      <c r="A436" s="25"/>
     </row>
     <row r="437">
-      <c r="A437" s="27"/>
+      <c r="A437" s="25"/>
     </row>
     <row r="438">
-      <c r="A438" s="27"/>
+      <c r="A438" s="25"/>
     </row>
     <row r="439">
-      <c r="A439" s="27"/>
+      <c r="A439" s="25"/>
     </row>
     <row r="440">
-      <c r="A440" s="27"/>
+      <c r="A440" s="25"/>
     </row>
     <row r="441">
-      <c r="A441" s="27"/>
+      <c r="A441" s="25"/>
     </row>
     <row r="442">
-      <c r="A442" s="27"/>
+      <c r="A442" s="25"/>
     </row>
     <row r="443">
-      <c r="A443" s="27"/>
+      <c r="A443" s="25"/>
     </row>
     <row r="444">
-      <c r="A444" s="27"/>
+      <c r="A444" s="25"/>
     </row>
     <row r="445">
-      <c r="A445" s="27"/>
+      <c r="A445" s="25"/>
     </row>
     <row r="446">
-      <c r="A446" s="27"/>
+      <c r="A446" s="25"/>
     </row>
     <row r="447">
-      <c r="A447" s="27"/>
+      <c r="A447" s="25"/>
     </row>
     <row r="448">
-      <c r="A448" s="27"/>
+      <c r="A448" s="25"/>
     </row>
     <row r="449">
-      <c r="A449" s="27"/>
+      <c r="A449" s="25"/>
     </row>
     <row r="450">
-      <c r="A450" s="27"/>
+      <c r="A450" s="25"/>
     </row>
     <row r="451">
-      <c r="A451" s="27"/>
+      <c r="A451" s="25"/>
     </row>
     <row r="452">
-      <c r="A452" s="27"/>
+      <c r="A452" s="25"/>
     </row>
     <row r="453">
-      <c r="A453" s="27"/>
+      <c r="A453" s="25"/>
     </row>
     <row r="454">
-      <c r="A454" s="27"/>
+      <c r="A454" s="25"/>
     </row>
     <row r="455">
-      <c r="A455" s="27"/>
+      <c r="A455" s="25"/>
     </row>
     <row r="456">
-      <c r="A456" s="27"/>
+      <c r="A456" s="25"/>
     </row>
     <row r="457">
-      <c r="A457" s="27"/>
+      <c r="A457" s="25"/>
     </row>
     <row r="458">
-      <c r="A458" s="27"/>
+      <c r="A458" s="25"/>
     </row>
     <row r="459">
-      <c r="A459" s="27"/>
+      <c r="A459" s="25"/>
     </row>
     <row r="460">
-      <c r="A460" s="27"/>
+      <c r="A460" s="25"/>
     </row>
     <row r="461">
-      <c r="A461" s="27"/>
+      <c r="A461" s="25"/>
     </row>
     <row r="462">
-      <c r="A462" s="27"/>
+      <c r="A462" s="25"/>
     </row>
     <row r="463">
-      <c r="A463" s="27"/>
+      <c r="A463" s="25"/>
     </row>
     <row r="464">
-      <c r="A464" s="27"/>
+      <c r="A464" s="25"/>
     </row>
     <row r="465">
-      <c r="A465" s="27"/>
+      <c r="A465" s="25"/>
     </row>
     <row r="466">
-      <c r="A466" s="27"/>
+      <c r="A466" s="25"/>
     </row>
     <row r="467">
-      <c r="A467" s="27"/>
+      <c r="A467" s="25"/>
     </row>
     <row r="468">
-      <c r="A468" s="27"/>
+      <c r="A468" s="25"/>
     </row>
     <row r="469">
-      <c r="A469" s="27"/>
+      <c r="A469" s="25"/>
     </row>
     <row r="470">
-      <c r="A470" s="27"/>
+      <c r="A470" s="25"/>
     </row>
     <row r="471">
-      <c r="A471" s="27"/>
+      <c r="A471" s="25"/>
     </row>
     <row r="472">
-      <c r="A472" s="27"/>
+      <c r="A472" s="25"/>
     </row>
     <row r="473">
-      <c r="A473" s="27"/>
+      <c r="A473" s="25"/>
     </row>
     <row r="474">
-      <c r="A474" s="27"/>
+      <c r="A474" s="25"/>
     </row>
     <row r="475">
-      <c r="A475" s="27"/>
+      <c r="A475" s="25"/>
     </row>
     <row r="476">
-      <c r="A476" s="27"/>
+      <c r="A476" s="25"/>
     </row>
     <row r="477">
-      <c r="A477" s="27"/>
+      <c r="A477" s="25"/>
     </row>
     <row r="478">
-      <c r="A478" s="27"/>
+      <c r="A478" s="25"/>
     </row>
     <row r="479">
-      <c r="A479" s="27"/>
+      <c r="A479" s="25"/>
     </row>
     <row r="480">
-      <c r="A480" s="27"/>
+      <c r="A480" s="25"/>
     </row>
     <row r="481">
-      <c r="A481" s="27"/>
+      <c r="A481" s="25"/>
     </row>
     <row r="482">
-      <c r="A482" s="27"/>
+      <c r="A482" s="25"/>
     </row>
     <row r="483">
-      <c r="A483" s="27"/>
+      <c r="A483" s="25"/>
     </row>
     <row r="484">
-      <c r="A484" s="27"/>
+      <c r="A484" s="25"/>
     </row>
     <row r="485">
-      <c r="A485" s="27"/>
+      <c r="A485" s="25"/>
     </row>
     <row r="486">
-      <c r="A486" s="27"/>
+      <c r="A486" s="25"/>
     </row>
     <row r="487">
-      <c r="A487" s="27"/>
+      <c r="A487" s="25"/>
     </row>
     <row r="488">
-      <c r="A488" s="27"/>
+      <c r="A488" s="25"/>
     </row>
     <row r="489">
-      <c r="A489" s="27"/>
+      <c r="A489" s="25"/>
     </row>
     <row r="490">
-      <c r="A490" s="27"/>
+      <c r="A490" s="25"/>
     </row>
     <row r="491">
-      <c r="A491" s="27"/>
+      <c r="A491" s="25"/>
     </row>
     <row r="492">
-      <c r="A492" s="27"/>
+      <c r="A492" s="25"/>
     </row>
     <row r="493">
-      <c r="A493" s="27"/>
+      <c r="A493" s="25"/>
     </row>
     <row r="494">
-      <c r="A494" s="27"/>
+      <c r="A494" s="25"/>
     </row>
     <row r="495">
-      <c r="A495" s="27"/>
+      <c r="A495" s="25"/>
     </row>
     <row r="496">
-      <c r="A496" s="27"/>
+      <c r="A496" s="25"/>
     </row>
     <row r="497">
-      <c r="A497" s="27"/>
+      <c r="A497" s="25"/>
     </row>
     <row r="498">
-      <c r="A498" s="27"/>
+      <c r="A498" s="25"/>
     </row>
     <row r="499">
-      <c r="A499" s="27"/>
+      <c r="A499" s="25"/>
     </row>
     <row r="500">
-      <c r="A500" s="27"/>
+      <c r="A500" s="25"/>
     </row>
     <row r="501">
-      <c r="A501" s="27"/>
+      <c r="A501" s="25"/>
     </row>
     <row r="502">
-      <c r="A502" s="27"/>
+      <c r="A502" s="25"/>
     </row>
     <row r="503">
-      <c r="A503" s="27"/>
+      <c r="A503" s="25"/>
     </row>
     <row r="504">
-      <c r="A504" s="27"/>
+      <c r="A504" s="25"/>
     </row>
     <row r="505">
-      <c r="A505" s="27"/>
+      <c r="A505" s="25"/>
     </row>
     <row r="506">
-      <c r="A506" s="27"/>
+      <c r="A506" s="25"/>
     </row>
     <row r="507">
-      <c r="A507" s="27"/>
+      <c r="A507" s="25"/>
     </row>
     <row r="508">
-      <c r="A508" s="27"/>
+      <c r="A508" s="25"/>
     </row>
     <row r="509">
-      <c r="A509" s="27"/>
+      <c r="A509" s="25"/>
     </row>
     <row r="510">
-      <c r="A510" s="27"/>
+      <c r="A510" s="25"/>
     </row>
     <row r="511">
-      <c r="A511" s="27"/>
+      <c r="A511" s="25"/>
     </row>
     <row r="512">
-      <c r="A512" s="27"/>
+      <c r="A512" s="25"/>
     </row>
     <row r="513">
-      <c r="A513" s="27"/>
+      <c r="A513" s="25"/>
     </row>
     <row r="514">
-      <c r="A514" s="27"/>
+      <c r="A514" s="25"/>
     </row>
     <row r="515">
-      <c r="A515" s="27"/>
+      <c r="A515" s="25"/>
     </row>
     <row r="516">
-      <c r="A516" s="27"/>
+      <c r="A516" s="25"/>
     </row>
     <row r="517">
-      <c r="A517" s="27"/>
+      <c r="A517" s="25"/>
     </row>
     <row r="518">
-      <c r="A518" s="27"/>
+      <c r="A518" s="25"/>
     </row>
     <row r="519">
-      <c r="A519" s="27"/>
+      <c r="A519" s="25"/>
     </row>
     <row r="520">
-      <c r="A520" s="27"/>
+      <c r="A520" s="25"/>
     </row>
     <row r="521">
-      <c r="A521" s="27"/>
+      <c r="A521" s="25"/>
     </row>
     <row r="522">
-      <c r="A522" s="27"/>
+      <c r="A522" s="25"/>
     </row>
     <row r="523">
-      <c r="A523" s="27"/>
+      <c r="A523" s="25"/>
     </row>
     <row r="524">
-      <c r="A524" s="27"/>
+      <c r="A524" s="25"/>
     </row>
     <row r="525">
-      <c r="A525" s="27"/>
+      <c r="A525" s="25"/>
     </row>
     <row r="526">
-      <c r="A526" s="27"/>
+      <c r="A526" s="25"/>
     </row>
     <row r="527">
-      <c r="A527" s="27"/>
+      <c r="A527" s="25"/>
     </row>
     <row r="528">
-      <c r="A528" s="27"/>
+      <c r="A528" s="25"/>
     </row>
     <row r="529">
-      <c r="A529" s="27"/>
+      <c r="A529" s="25"/>
     </row>
     <row r="530">
-      <c r="A530" s="27"/>
+      <c r="A530" s="25"/>
     </row>
     <row r="531">
-      <c r="A531" s="27"/>
+      <c r="A531" s="25"/>
     </row>
     <row r="532">
-      <c r="A532" s="27"/>
+      <c r="A532" s="25"/>
     </row>
     <row r="533">
-      <c r="A533" s="27"/>
+      <c r="A533" s="25"/>
     </row>
     <row r="534">
-      <c r="A534" s="27"/>
+      <c r="A534" s="25"/>
     </row>
     <row r="535">
-      <c r="A535" s="27"/>
+      <c r="A535" s="25"/>
     </row>
     <row r="536">
-      <c r="A536" s="27"/>
+      <c r="A536" s="25"/>
     </row>
     <row r="537">
-      <c r="A537" s="27"/>
+      <c r="A537" s="25"/>
     </row>
     <row r="538">
-      <c r="A538" s="27"/>
+      <c r="A538" s="25"/>
     </row>
     <row r="539">
-      <c r="A539" s="27"/>
+      <c r="A539" s="25"/>
     </row>
     <row r="540">
-      <c r="A540" s="27"/>
+      <c r="A540" s="25"/>
     </row>
     <row r="541">
-      <c r="A541" s="27"/>
+      <c r="A541" s="25"/>
     </row>
     <row r="542">
-      <c r="A542" s="27"/>
+      <c r="A542" s="25"/>
     </row>
     <row r="543">
-      <c r="A543" s="27"/>
+      <c r="A543" s="25"/>
     </row>
     <row r="544">
-      <c r="A544" s="27"/>
+      <c r="A544" s="25"/>
     </row>
     <row r="545">
-      <c r="A545" s="27"/>
+      <c r="A545" s="25"/>
     </row>
     <row r="546">
-      <c r="A546" s="27"/>
+      <c r="A546" s="25"/>
     </row>
     <row r="547">
-      <c r="A547" s="27"/>
+      <c r="A547" s="25"/>
     </row>
     <row r="548">
-      <c r="A548" s="27"/>
+      <c r="A548" s="25"/>
     </row>
     <row r="549">
-      <c r="A549" s="27"/>
+      <c r="A549" s="25"/>
     </row>
     <row r="550">
-      <c r="A550" s="27"/>
+      <c r="A550" s="25"/>
     </row>
     <row r="551">
-      <c r="A551" s="27"/>
+      <c r="A551" s="25"/>
     </row>
     <row r="552">
-      <c r="A552" s="27"/>
+      <c r="A552" s="25"/>
     </row>
     <row r="553">
-      <c r="A553" s="27"/>
+      <c r="A553" s="25"/>
     </row>
     <row r="554">
-      <c r="A554" s="27"/>
+      <c r="A554" s="25"/>
     </row>
     <row r="555">
-      <c r="A555" s="27"/>
+      <c r="A555" s="25"/>
     </row>
     <row r="556">
-      <c r="A556" s="27"/>
+      <c r="A556" s="25"/>
     </row>
     <row r="557">
-      <c r="A557" s="27"/>
+      <c r="A557" s="25"/>
     </row>
     <row r="558">
-      <c r="A558" s="27"/>
+      <c r="A558" s="25"/>
     </row>
     <row r="559">
-      <c r="A559" s="27"/>
+      <c r="A559" s="25"/>
     </row>
     <row r="560">
-      <c r="A560" s="27"/>
+      <c r="A560" s="25"/>
     </row>
     <row r="561">
-      <c r="A561" s="27"/>
+      <c r="A561" s="25"/>
     </row>
     <row r="562">
-      <c r="A562" s="27"/>
+      <c r="A562" s="25"/>
     </row>
     <row r="563">
-      <c r="A563" s="27"/>
+      <c r="A563" s="25"/>
     </row>
     <row r="564">
-      <c r="A564" s="27"/>
+      <c r="A564" s="25"/>
     </row>
     <row r="565">
-      <c r="A565" s="27"/>
+      <c r="A565" s="25"/>
     </row>
     <row r="566">
-      <c r="A566" s="27"/>
+      <c r="A566" s="25"/>
     </row>
     <row r="567">
-      <c r="A567" s="27"/>
+      <c r="A567" s="25"/>
     </row>
     <row r="568">
-      <c r="A568" s="27"/>
+      <c r="A568" s="25"/>
     </row>
     <row r="569">
-      <c r="A569" s="27"/>
+      <c r="A569" s="25"/>
     </row>
     <row r="570">
-      <c r="A570" s="27"/>
+      <c r="A570" s="25"/>
     </row>
     <row r="571">
-      <c r="A571" s="27"/>
+      <c r="A571" s="25"/>
     </row>
     <row r="572">
-      <c r="A572" s="27"/>
+      <c r="A572" s="25"/>
     </row>
     <row r="573">
-      <c r="A573" s="27"/>
+      <c r="A573" s="25"/>
     </row>
     <row r="574">
-      <c r="A574" s="27"/>
+      <c r="A574" s="25"/>
     </row>
     <row r="575">
-      <c r="A575" s="27"/>
+      <c r="A575" s="25"/>
     </row>
     <row r="576">
-      <c r="A576" s="27"/>
+      <c r="A576" s="25"/>
     </row>
     <row r="577">
-      <c r="A577" s="27"/>
+      <c r="A577" s="25"/>
     </row>
     <row r="578">
-      <c r="A578" s="27"/>
+      <c r="A578" s="25"/>
     </row>
     <row r="579">
-      <c r="A579" s="27"/>
+      <c r="A579" s="25"/>
     </row>
     <row r="580">
-      <c r="A580" s="27"/>
+      <c r="A580" s="25"/>
     </row>
     <row r="581">
-      <c r="A581" s="27"/>
+      <c r="A581" s="25"/>
     </row>
     <row r="582">
-      <c r="A582" s="27"/>
+      <c r="A582" s="25"/>
     </row>
     <row r="583">
-      <c r="A583" s="27"/>
+      <c r="A583" s="25"/>
     </row>
     <row r="584">
-      <c r="A584" s="27"/>
+      <c r="A584" s="25"/>
     </row>
     <row r="585">
-      <c r="A585" s="27"/>
+      <c r="A585" s="25"/>
     </row>
     <row r="586">
-      <c r="A586" s="27"/>
+      <c r="A586" s="25"/>
     </row>
     <row r="587">
-      <c r="A587" s="27"/>
+      <c r="A587" s="25"/>
     </row>
     <row r="588">
-      <c r="A588" s="27"/>
+      <c r="A588" s="25"/>
     </row>
     <row r="589">
-      <c r="A589" s="27"/>
+      <c r="A589" s="25"/>
     </row>
     <row r="590">
-      <c r="A590" s="27"/>
+      <c r="A590" s="25"/>
     </row>
     <row r="591">
-      <c r="A591" s="27"/>
+      <c r="A591" s="25"/>
     </row>
     <row r="592">
-      <c r="A592" s="27"/>
+      <c r="A592" s="25"/>
     </row>
     <row r="593">
-      <c r="A593" s="27"/>
+      <c r="A593" s="25"/>
     </row>
     <row r="594">
-      <c r="A594" s="27"/>
+      <c r="A594" s="25"/>
     </row>
     <row r="595">
-      <c r="A595" s="27"/>
+      <c r="A595" s="25"/>
     </row>
     <row r="596">
-      <c r="A596" s="27"/>
+      <c r="A596" s="25"/>
     </row>
     <row r="597">
-      <c r="A597" s="27"/>
+      <c r="A597" s="25"/>
     </row>
     <row r="598">
-      <c r="A598" s="27"/>
+      <c r="A598" s="25"/>
     </row>
     <row r="599">
-      <c r="A599" s="27"/>
+      <c r="A599" s="25"/>
     </row>
     <row r="600">
-      <c r="A600" s="27"/>
+      <c r="A600" s="25"/>
     </row>
     <row r="601">
-      <c r="A601" s="27"/>
+      <c r="A601" s="25"/>
     </row>
     <row r="602">
-      <c r="A602" s="27"/>
+      <c r="A602" s="25"/>
     </row>
     <row r="603">
-      <c r="A603" s="27"/>
+      <c r="A603" s="25"/>
     </row>
     <row r="604">
-      <c r="A604" s="27"/>
+      <c r="A604" s="25"/>
     </row>
     <row r="605">
-      <c r="A605" s="27"/>
+      <c r="A605" s="25"/>
     </row>
     <row r="606">
-      <c r="A606" s="27"/>
+      <c r="A606" s="25"/>
     </row>
     <row r="607">
-      <c r="A607" s="27"/>
+      <c r="A607" s="25"/>
     </row>
     <row r="608">
-      <c r="A608" s="27"/>
+      <c r="A608" s="25"/>
     </row>
     <row r="609">
-      <c r="A609" s="27"/>
+      <c r="A609" s="25"/>
     </row>
     <row r="610">
-      <c r="A610" s="27"/>
+      <c r="A610" s="25"/>
     </row>
     <row r="611">
-      <c r="A611" s="27"/>
+      <c r="A611" s="25"/>
     </row>
     <row r="612">
-      <c r="A612" s="27"/>
+      <c r="A612" s="25"/>
     </row>
     <row r="613">
-      <c r="A613" s="27"/>
+      <c r="A613" s="25"/>
     </row>
     <row r="614">
-      <c r="A614" s="27"/>
+      <c r="A614" s="25"/>
     </row>
     <row r="615">
-      <c r="A615" s="27"/>
+      <c r="A615" s="25"/>
     </row>
     <row r="616">
-      <c r="A616" s="27"/>
+      <c r="A616" s="25"/>
     </row>
     <row r="617">
-      <c r="A617" s="27"/>
+      <c r="A617" s="25"/>
     </row>
     <row r="618">
-      <c r="A618" s="27"/>
+      <c r="A618" s="25"/>
     </row>
     <row r="619">
-      <c r="A619" s="27"/>
+      <c r="A619" s="25"/>
     </row>
     <row r="620">
-      <c r="A620" s="27"/>
+      <c r="A620" s="25"/>
     </row>
     <row r="621">
-      <c r="A621" s="27"/>
+      <c r="A621" s="25"/>
     </row>
     <row r="622">
-      <c r="A622" s="27"/>
+      <c r="A622" s="25"/>
     </row>
     <row r="623">
-      <c r="A623" s="27"/>
+      <c r="A623" s="25"/>
     </row>
     <row r="624">
-      <c r="A624" s="27"/>
+      <c r="A624" s="25"/>
     </row>
     <row r="625">
-      <c r="A625" s="27"/>
+      <c r="A625" s="25"/>
     </row>
     <row r="626">
-      <c r="A626" s="27"/>
+      <c r="A626" s="25"/>
     </row>
     <row r="627">
-      <c r="A627" s="27"/>
+      <c r="A627" s="25"/>
     </row>
     <row r="628">
-      <c r="A628" s="27"/>
+      <c r="A628" s="25"/>
     </row>
     <row r="629">
-      <c r="A629" s="27"/>
+      <c r="A629" s="25"/>
     </row>
     <row r="630">
-      <c r="A630" s="27"/>
+      <c r="A630" s="25"/>
     </row>
     <row r="631">
-      <c r="A631" s="27"/>
+      <c r="A631" s="25"/>
     </row>
     <row r="632">
-      <c r="A632" s="27"/>
+      <c r="A632" s="25"/>
     </row>
     <row r="633">
-      <c r="A633" s="27"/>
+      <c r="A633" s="25"/>
     </row>
     <row r="634">
-      <c r="A634" s="27"/>
+      <c r="A634" s="25"/>
     </row>
     <row r="635">
-      <c r="A635" s="27"/>
+      <c r="A635" s="25"/>
     </row>
     <row r="636">
-      <c r="A636" s="27"/>
+      <c r="A636" s="25"/>
     </row>
     <row r="637">
-      <c r="A637" s="27"/>
+      <c r="A637" s="25"/>
     </row>
     <row r="638">
-      <c r="A638" s="27"/>
+      <c r="A638" s="25"/>
     </row>
     <row r="639">
-      <c r="A639" s="27"/>
+      <c r="A639" s="25"/>
     </row>
     <row r="640">
-      <c r="A640" s="27"/>
+      <c r="A640" s="25"/>
     </row>
     <row r="641">
-      <c r="A641" s="27"/>
+      <c r="A641" s="25"/>
     </row>
     <row r="642">
-      <c r="A642" s="27"/>
+      <c r="A642" s="25"/>
     </row>
     <row r="643">
-      <c r="A643" s="27"/>
+      <c r="A643" s="25"/>
     </row>
     <row r="644">
-      <c r="A644" s="27"/>
+      <c r="A644" s="25"/>
     </row>
     <row r="645">
-      <c r="A645" s="27"/>
+      <c r="A645" s="25"/>
     </row>
     <row r="646">
-      <c r="A646" s="27"/>
+      <c r="A646" s="25"/>
     </row>
     <row r="647">
-      <c r="A647" s="27"/>
+      <c r="A647" s="25"/>
     </row>
     <row r="648">
-      <c r="A648" s="27"/>
+      <c r="A648" s="25"/>
     </row>
     <row r="649">
-      <c r="A649" s="27"/>
+      <c r="A649" s="25"/>
     </row>
     <row r="650">
-      <c r="A650" s="27"/>
+      <c r="A650" s="25"/>
     </row>
     <row r="651">
-      <c r="A651" s="27"/>
+      <c r="A651" s="25"/>
     </row>
     <row r="652">
-      <c r="A652" s="27"/>
+      <c r="A652" s="25"/>
     </row>
     <row r="653">
-      <c r="A653" s="27"/>
+      <c r="A653" s="25"/>
     </row>
     <row r="654">
-      <c r="A654" s="27"/>
+      <c r="A654" s="25"/>
     </row>
     <row r="655">
-      <c r="A655" s="27"/>
+      <c r="A655" s="25"/>
     </row>
     <row r="656">
-      <c r="A656" s="27"/>
+      <c r="A656" s="25"/>
     </row>
     <row r="657">
-      <c r="A657" s="27"/>
+      <c r="A657" s="25"/>
     </row>
     <row r="658">
-      <c r="A658" s="27"/>
+      <c r="A658" s="25"/>
     </row>
     <row r="659">
-      <c r="A659" s="27"/>
+      <c r="A659" s="25"/>
     </row>
     <row r="660">
-      <c r="A660" s="27"/>
+      <c r="A660" s="25"/>
     </row>
     <row r="661">
-      <c r="A661" s="27"/>
+      <c r="A661" s="25"/>
     </row>
     <row r="662">
-      <c r="A662" s="27"/>
+      <c r="A662" s="25"/>
     </row>
     <row r="663">
-      <c r="A663" s="27"/>
+      <c r="A663" s="25"/>
     </row>
     <row r="664">
-      <c r="A664" s="27"/>
+      <c r="A664" s="25"/>
     </row>
     <row r="665">
-      <c r="A665" s="27"/>
+      <c r="A665" s="25"/>
     </row>
     <row r="666">
-      <c r="A666" s="27"/>
+      <c r="A666" s="25"/>
     </row>
     <row r="667">
-      <c r="A667" s="27"/>
+      <c r="A667" s="25"/>
     </row>
     <row r="668">
-      <c r="A668" s="27"/>
+      <c r="A668" s="25"/>
     </row>
     <row r="669">
-      <c r="A669" s="27"/>
+      <c r="A669" s="25"/>
     </row>
     <row r="670">
-      <c r="A670" s="27"/>
+      <c r="A670" s="25"/>
     </row>
     <row r="671">
-      <c r="A671" s="27"/>
+      <c r="A671" s="25"/>
     </row>
     <row r="672">
-      <c r="A672" s="27"/>
+      <c r="A672" s="25"/>
     </row>
     <row r="673">
-      <c r="A673" s="27"/>
+      <c r="A673" s="25"/>
     </row>
     <row r="674">
-      <c r="A674" s="27"/>
+      <c r="A674" s="25"/>
     </row>
     <row r="675">
-      <c r="A675" s="27"/>
+      <c r="A675" s="25"/>
     </row>
     <row r="676">
-      <c r="A676" s="27"/>
+      <c r="A676" s="25"/>
     </row>
     <row r="677">
-      <c r="A677" s="27"/>
+      <c r="A677" s="25"/>
     </row>
     <row r="678">
-      <c r="A678" s="27"/>
+      <c r="A678" s="25"/>
     </row>
     <row r="679">
-      <c r="A679" s="27"/>
+      <c r="A679" s="25"/>
     </row>
     <row r="680">
-      <c r="A680" s="27"/>
+      <c r="A680" s="25"/>
     </row>
     <row r="681">
-      <c r="A681" s="27"/>
+      <c r="A681" s="25"/>
     </row>
     <row r="682">
-      <c r="A682" s="27"/>
+      <c r="A682" s="25"/>
     </row>
     <row r="683">
-      <c r="A683" s="27"/>
+      <c r="A683" s="25"/>
     </row>
     <row r="684">
-      <c r="A684" s="27"/>
+      <c r="A684" s="25"/>
     </row>
     <row r="685">
-      <c r="A685" s="27"/>
+      <c r="A685" s="25"/>
     </row>
     <row r="686">
-      <c r="A686" s="27"/>
+      <c r="A686" s="25"/>
     </row>
     <row r="687">
-      <c r="A687" s="27"/>
+      <c r="A687" s="25"/>
     </row>
     <row r="688">
-      <c r="A688" s="27"/>
+      <c r="A688" s="25"/>
     </row>
     <row r="689">
-      <c r="A689" s="27"/>
+      <c r="A689" s="25"/>
     </row>
     <row r="690">
-      <c r="A690" s="27"/>
+      <c r="A690" s="25"/>
     </row>
     <row r="691">
-      <c r="A691" s="27"/>
+      <c r="A691" s="25"/>
     </row>
     <row r="692">
-      <c r="A692" s="27"/>
+      <c r="A692" s="25"/>
     </row>
     <row r="693">
-      <c r="A693" s="27"/>
+      <c r="A693" s="25"/>
     </row>
     <row r="694">
-      <c r="A694" s="27"/>
+      <c r="A694" s="25"/>
     </row>
     <row r="695">
-      <c r="A695" s="27"/>
+      <c r="A695" s="25"/>
     </row>
     <row r="696">
-      <c r="A696" s="27"/>
+      <c r="A696" s="25"/>
     </row>
     <row r="697">
-      <c r="A697" s="27"/>
+      <c r="A697" s="25"/>
     </row>
     <row r="698">
-      <c r="A698" s="27"/>
+      <c r="A698" s="25"/>
     </row>
     <row r="699">
-      <c r="A699" s="27"/>
+      <c r="A699" s="25"/>
     </row>
     <row r="700">
-      <c r="A700" s="27"/>
+      <c r="A700" s="25"/>
     </row>
     <row r="701">
-      <c r="A701" s="27"/>
+      <c r="A701" s="25"/>
     </row>
     <row r="702">
-      <c r="A702" s="27"/>
+      <c r="A702" s="25"/>
     </row>
     <row r="703">
-      <c r="A703" s="27"/>
+      <c r="A703" s="25"/>
     </row>
     <row r="704">
-      <c r="A704" s="27"/>
+      <c r="A704" s="25"/>
     </row>
     <row r="705">
-      <c r="A705" s="27"/>
+      <c r="A705" s="25"/>
     </row>
     <row r="706">
-      <c r="A706" s="27"/>
+      <c r="A706" s="25"/>
     </row>
     <row r="707">
-      <c r="A707" s="27"/>
+      <c r="A707" s="25"/>
     </row>
     <row r="708">
-      <c r="A708" s="27"/>
+      <c r="A708" s="25"/>
     </row>
     <row r="709">
-      <c r="A709" s="27"/>
+      <c r="A709" s="25"/>
     </row>
     <row r="710">
-      <c r="A710" s="27"/>
+      <c r="A710" s="25"/>
     </row>
     <row r="711">
-      <c r="A711" s="27"/>
+      <c r="A711" s="25"/>
     </row>
     <row r="712">
-      <c r="A712" s="27"/>
+      <c r="A712" s="25"/>
     </row>
     <row r="713">
-      <c r="A713" s="27"/>
+      <c r="A713" s="25"/>
     </row>
     <row r="714">
-      <c r="A714" s="27"/>
+      <c r="A714" s="25"/>
     </row>
     <row r="715">
-      <c r="A715" s="27"/>
+      <c r="A715" s="25"/>
     </row>
     <row r="716">
-      <c r="A716" s="27"/>
+      <c r="A716" s="25"/>
     </row>
     <row r="717">
-      <c r="A717" s="27"/>
+      <c r="A717" s="25"/>
     </row>
     <row r="718">
-      <c r="A718" s="27"/>
+      <c r="A718" s="25"/>
     </row>
     <row r="719">
-      <c r="A719" s="27"/>
+      <c r="A719" s="25"/>
     </row>
     <row r="720">
-      <c r="A720" s="27"/>
+      <c r="A720" s="25"/>
     </row>
     <row r="721">
-      <c r="A721" s="27"/>
+      <c r="A721" s="25"/>
     </row>
     <row r="722">
-      <c r="A722" s="27"/>
+      <c r="A722" s="25"/>
     </row>
     <row r="723">
-      <c r="A723" s="27"/>
+      <c r="A723" s="25"/>
     </row>
     <row r="724">
-      <c r="A724" s="27"/>
+      <c r="A724" s="25"/>
     </row>
     <row r="725">
-      <c r="A725" s="27"/>
+      <c r="A725" s="25"/>
     </row>
     <row r="726">
-      <c r="A726" s="27"/>
+      <c r="A726" s="25"/>
     </row>
     <row r="727">
-      <c r="A727" s="27"/>
+      <c r="A727" s="25"/>
     </row>
     <row r="728">
-      <c r="A728" s="27"/>
+      <c r="A728" s="25"/>
     </row>
     <row r="729">
-      <c r="A729" s="27"/>
+      <c r="A729" s="25"/>
     </row>
     <row r="730">
-      <c r="A730" s="27"/>
+      <c r="A730" s="25"/>
     </row>
     <row r="731">
-      <c r="A731" s="27"/>
+      <c r="A731" s="25"/>
     </row>
     <row r="732">
-      <c r="A732" s="27"/>
+      <c r="A732" s="25"/>
     </row>
     <row r="733">
-      <c r="A733" s="27"/>
+      <c r="A733" s="25"/>
     </row>
     <row r="734">
-      <c r="A734" s="27"/>
+      <c r="A734" s="25"/>
     </row>
     <row r="735">
-      <c r="A735" s="27"/>
+      <c r="A735" s="25"/>
     </row>
     <row r="736">
-      <c r="A736" s="27"/>
+      <c r="A736" s="25"/>
     </row>
     <row r="737">
-      <c r="A737" s="27"/>
+      <c r="A737" s="25"/>
     </row>
     <row r="738">
-      <c r="A738" s="27"/>
+      <c r="A738" s="25"/>
     </row>
     <row r="739">
-      <c r="A739" s="27"/>
+      <c r="A739" s="25"/>
     </row>
     <row r="740">
-      <c r="A740" s="27"/>
+      <c r="A740" s="25"/>
     </row>
     <row r="741">
-      <c r="A741" s="27"/>
+      <c r="A741" s="25"/>
     </row>
     <row r="742">
-      <c r="A742" s="27"/>
+      <c r="A742" s="25"/>
     </row>
     <row r="743">
-      <c r="A743" s="27"/>
+      <c r="A743" s="25"/>
     </row>
     <row r="744">
-      <c r="A744" s="27"/>
+      <c r="A744" s="25"/>
     </row>
     <row r="745">
-      <c r="A745" s="27"/>
+      <c r="A745" s="25"/>
     </row>
     <row r="746">
-      <c r="A746" s="27"/>
+      <c r="A746" s="25"/>
     </row>
     <row r="747">
-      <c r="A747" s="27"/>
+      <c r="A747" s="25"/>
     </row>
     <row r="748">
-      <c r="A748" s="27"/>
+      <c r="A748" s="25"/>
     </row>
     <row r="749">
-      <c r="A749" s="27"/>
+      <c r="A749" s="25"/>
     </row>
     <row r="750">
-      <c r="A750" s="27"/>
+      <c r="A750" s="25"/>
     </row>
     <row r="751">
-      <c r="A751" s="27"/>
+      <c r="A751" s="25"/>
     </row>
     <row r="752">
-      <c r="A752" s="27"/>
+      <c r="A752" s="25"/>
     </row>
     <row r="753">
-      <c r="A753" s="27"/>
+      <c r="A753" s="25"/>
     </row>
     <row r="754">
-      <c r="A754" s="27"/>
+      <c r="A754" s="25"/>
     </row>
     <row r="755">
-      <c r="A755" s="27"/>
+      <c r="A755" s="25"/>
     </row>
     <row r="756">
-      <c r="A756" s="27"/>
+      <c r="A756" s="25"/>
     </row>
     <row r="757">
-      <c r="A757" s="27"/>
+      <c r="A757" s="25"/>
     </row>
     <row r="758">
-      <c r="A758" s="27"/>
+      <c r="A758" s="25"/>
     </row>
     <row r="759">
-      <c r="A759" s="27"/>
+      <c r="A759" s="25"/>
     </row>
     <row r="760">
-      <c r="A760" s="27"/>
+      <c r="A760" s="25"/>
     </row>
     <row r="761">
-      <c r="A761" s="27"/>
+      <c r="A761" s="25"/>
     </row>
     <row r="762">
-      <c r="A762" s="27"/>
+      <c r="A762" s="25"/>
     </row>
     <row r="763">
-      <c r="A763" s="27"/>
+      <c r="A763" s="25"/>
     </row>
     <row r="764">
-      <c r="A764" s="27"/>
+      <c r="A764" s="25"/>
     </row>
     <row r="765">
-      <c r="A765" s="27"/>
+      <c r="A765" s="25"/>
     </row>
     <row r="766">
-      <c r="A766" s="27"/>
+      <c r="A766" s="25"/>
     </row>
     <row r="767">
-      <c r="A767" s="27"/>
+      <c r="A767" s="25"/>
     </row>
     <row r="768">
-      <c r="A768" s="27"/>
+      <c r="A768" s="25"/>
     </row>
     <row r="769">
-      <c r="A769" s="27"/>
+      <c r="A769" s="25"/>
     </row>
     <row r="770">
-      <c r="A770" s="27"/>
+      <c r="A770" s="25"/>
     </row>
     <row r="771">
-      <c r="A771" s="27"/>
+      <c r="A771" s="25"/>
     </row>
     <row r="772">
-      <c r="A772" s="27"/>
+      <c r="A772" s="25"/>
     </row>
     <row r="773">
-      <c r="A773" s="27"/>
+      <c r="A773" s="25"/>
     </row>
     <row r="774">
-      <c r="A774" s="27"/>
+      <c r="A774" s="25"/>
     </row>
     <row r="775">
-      <c r="A775" s="27"/>
+      <c r="A775" s="25"/>
     </row>
     <row r="776">
-      <c r="A776" s="27"/>
+      <c r="A776" s="25"/>
     </row>
     <row r="777">
-      <c r="A777" s="27"/>
+      <c r="A777" s="25"/>
     </row>
     <row r="778">
-      <c r="A778" s="27"/>
+      <c r="A778" s="25"/>
     </row>
     <row r="779">
-      <c r="A779" s="27"/>
+      <c r="A779" s="25"/>
     </row>
     <row r="780">
-      <c r="A780" s="27"/>
+      <c r="A780" s="25"/>
     </row>
     <row r="781">
-      <c r="A781" s="27"/>
+      <c r="A781" s="25"/>
     </row>
     <row r="782">
-      <c r="A782" s="27"/>
+      <c r="A782" s="25"/>
     </row>
     <row r="783">
-      <c r="A783" s="27"/>
+      <c r="A783" s="25"/>
     </row>
     <row r="784">
-      <c r="A784" s="27"/>
+      <c r="A784" s="25"/>
     </row>
     <row r="785">
-      <c r="A785" s="27"/>
+      <c r="A785" s="25"/>
     </row>
     <row r="786">
-      <c r="A786" s="27"/>
+      <c r="A786" s="25"/>
     </row>
     <row r="787">
-      <c r="A787" s="27"/>
+      <c r="A787" s="25"/>
     </row>
     <row r="788">
-      <c r="A788" s="27"/>
+      <c r="A788" s="25"/>
     </row>
     <row r="789">
-      <c r="A789" s="27"/>
+      <c r="A789" s="25"/>
     </row>
     <row r="790">
-      <c r="A790" s="27"/>
+      <c r="A790" s="25"/>
     </row>
     <row r="791">
-      <c r="A791" s="27"/>
+      <c r="A791" s="25"/>
     </row>
     <row r="792">
-      <c r="A792" s="27"/>
+      <c r="A792" s="25"/>
     </row>
     <row r="793">
-      <c r="A793" s="27"/>
+      <c r="A793" s="25"/>
     </row>
     <row r="794">
-      <c r="A794" s="27"/>
+      <c r="A794" s="25"/>
     </row>
     <row r="795">
-      <c r="A795" s="27"/>
+      <c r="A795" s="25"/>
     </row>
     <row r="796">
-      <c r="A796" s="27"/>
+      <c r="A796" s="25"/>
     </row>
     <row r="797">
-      <c r="A797" s="27"/>
+      <c r="A797" s="25"/>
     </row>
     <row r="798">
-      <c r="A798" s="27"/>
+      <c r="A798" s="25"/>
     </row>
     <row r="799">
-      <c r="A799" s="27"/>
+      <c r="A799" s="25"/>
     </row>
     <row r="800">
-      <c r="A800" s="27"/>
+      <c r="A800" s="25"/>
     </row>
     <row r="801">
-      <c r="A801" s="27"/>
+      <c r="A801" s="25"/>
     </row>
     <row r="802">
-      <c r="A802" s="27"/>
+      <c r="A802" s="25"/>
     </row>
     <row r="803">
-      <c r="A803" s="27"/>
+      <c r="A803" s="25"/>
     </row>
     <row r="804">
-      <c r="A804" s="27"/>
+      <c r="A804" s="25"/>
     </row>
     <row r="805">
-      <c r="A805" s="27"/>
+      <c r="A805" s="25"/>
     </row>
     <row r="806">
-      <c r="A806" s="27"/>
+      <c r="A806" s="25"/>
     </row>
     <row r="807">
-      <c r="A807" s="27"/>
+      <c r="A807" s="25"/>
     </row>
     <row r="808">
-      <c r="A808" s="27"/>
+      <c r="A808" s="25"/>
     </row>
     <row r="809">
-      <c r="A809" s="27"/>
+      <c r="A809" s="25"/>
     </row>
     <row r="810">
-      <c r="A810" s="27"/>
+      <c r="A810" s="25"/>
     </row>
     <row r="811">
-      <c r="A811" s="27"/>
+      <c r="A811" s="25"/>
     </row>
     <row r="812">
-      <c r="A812" s="27"/>
+      <c r="A812" s="25"/>
     </row>
     <row r="813">
-      <c r="A813" s="27"/>
+      <c r="A813" s="25"/>
     </row>
     <row r="814">
-      <c r="A814" s="27"/>
+      <c r="A814" s="25"/>
     </row>
     <row r="815">
-      <c r="A815" s="27"/>
+      <c r="A815" s="25"/>
     </row>
     <row r="816">
-      <c r="A816" s="27"/>
+      <c r="A816" s="25"/>
     </row>
     <row r="817">
-      <c r="A817" s="27"/>
+      <c r="A817" s="25"/>
     </row>
     <row r="818">
-      <c r="A818" s="27"/>
+      <c r="A818" s="25"/>
     </row>
     <row r="819">
-      <c r="A819" s="27"/>
+      <c r="A819" s="25"/>
     </row>
     <row r="820">
-      <c r="A820" s="27"/>
+      <c r="A820" s="25"/>
     </row>
     <row r="821">
-      <c r="A821" s="27"/>
+      <c r="A821" s="25"/>
     </row>
     <row r="822">
-      <c r="A822" s="27"/>
+      <c r="A822" s="25"/>
     </row>
     <row r="823">
-      <c r="A823" s="27"/>
+      <c r="A823" s="25"/>
     </row>
     <row r="824">
-      <c r="A824" s="27"/>
+      <c r="A824" s="25"/>
     </row>
     <row r="825">
-      <c r="A825" s="27"/>
+      <c r="A825" s="25"/>
     </row>
     <row r="826">
-      <c r="A826" s="27"/>
+      <c r="A826" s="25"/>
     </row>
     <row r="827">
-      <c r="A827" s="27"/>
+      <c r="A827" s="25"/>
     </row>
     <row r="828">
-      <c r="A828" s="27"/>
+      <c r="A828" s="25"/>
     </row>
     <row r="829">
-      <c r="A829" s="27"/>
+      <c r="A829" s="25"/>
     </row>
     <row r="830">
-      <c r="A830" s="27"/>
+      <c r="A830" s="25"/>
     </row>
     <row r="831">
-      <c r="A831" s="27"/>
+      <c r="A831" s="25"/>
     </row>
     <row r="832">
-      <c r="A832" s="27"/>
+      <c r="A832" s="25"/>
     </row>
     <row r="833">
-      <c r="A833" s="27"/>
+      <c r="A833" s="25"/>
     </row>
     <row r="834">
-      <c r="A834" s="27"/>
+      <c r="A834" s="25"/>
     </row>
     <row r="835">
-      <c r="A835" s="27"/>
+      <c r="A835" s="25"/>
     </row>
     <row r="836">
-      <c r="A836" s="27"/>
+      <c r="A836" s="25"/>
     </row>
     <row r="837">
-      <c r="A837" s="27"/>
+      <c r="A837" s="25"/>
     </row>
     <row r="838">
-      <c r="A838" s="27"/>
+      <c r="A838" s="25"/>
     </row>
     <row r="839">
-      <c r="A839" s="27"/>
+      <c r="A839" s="25"/>
     </row>
     <row r="840">
-      <c r="A840" s="27"/>
+      <c r="A840" s="25"/>
     </row>
     <row r="841">
-      <c r="A841" s="27"/>
+      <c r="A841" s="25"/>
     </row>
     <row r="842">
-      <c r="A842" s="27"/>
+      <c r="A842" s="25"/>
     </row>
     <row r="843">
-      <c r="A843" s="27"/>
+      <c r="A843" s="25"/>
     </row>
     <row r="844">
-      <c r="A844" s="27"/>
+      <c r="A844" s="25"/>
     </row>
     <row r="845">
-      <c r="A845" s="27"/>
+      <c r="A845" s="25"/>
     </row>
     <row r="846">
-      <c r="A846" s="27"/>
+      <c r="A846" s="25"/>
     </row>
     <row r="847">
-      <c r="A847" s="27"/>
+      <c r="A847" s="25"/>
     </row>
     <row r="848">
-      <c r="A848" s="27"/>
+      <c r="A848" s="25"/>
     </row>
     <row r="849">
-      <c r="A849" s="27"/>
+      <c r="A849" s="25"/>
     </row>
     <row r="850">
-      <c r="A850" s="27"/>
+      <c r="A850" s="25"/>
     </row>
     <row r="851">
-      <c r="A851" s="27"/>
+      <c r="A851" s="25"/>
     </row>
     <row r="852">
-      <c r="A852" s="27"/>
+      <c r="A852" s="25"/>
     </row>
     <row r="853">
-      <c r="A853" s="27"/>
+      <c r="A853" s="25"/>
     </row>
     <row r="854">
-      <c r="A854" s="27"/>
+      <c r="A854" s="25"/>
     </row>
     <row r="855">
-      <c r="A855" s="27"/>
+      <c r="A855" s="25"/>
     </row>
     <row r="856">
-      <c r="A856" s="27"/>
+      <c r="A856" s="25"/>
     </row>
     <row r="857">
-      <c r="A857" s="27"/>
+      <c r="A857" s="25"/>
     </row>
     <row r="858">
-      <c r="A858" s="27"/>
+      <c r="A858" s="25"/>
     </row>
     <row r="859">
-      <c r="A859" s="27"/>
+      <c r="A859" s="25"/>
     </row>
     <row r="860">
-      <c r="A860" s="27"/>
+      <c r="A860" s="25"/>
     </row>
     <row r="861">
-      <c r="A861" s="27"/>
+      <c r="A861" s="25"/>
     </row>
     <row r="862">
-      <c r="A862" s="27"/>
+      <c r="A862" s="25"/>
     </row>
     <row r="863">
-      <c r="A863" s="27"/>
+      <c r="A863" s="25"/>
     </row>
     <row r="864">
-      <c r="A864" s="27"/>
+      <c r="A864" s="25"/>
     </row>
     <row r="865">
-      <c r="A865" s="27"/>
+      <c r="A865" s="25"/>
     </row>
     <row r="866">
-      <c r="A866" s="27"/>
+      <c r="A866" s="25"/>
     </row>
     <row r="867">
-      <c r="A867" s="27"/>
+      <c r="A867" s="25"/>
     </row>
     <row r="868">
-      <c r="A868" s="27"/>
+      <c r="A868" s="25"/>
     </row>
     <row r="869">
-      <c r="A869" s="27"/>
+      <c r="A869" s="25"/>
     </row>
     <row r="870">
-      <c r="A870" s="27"/>
+      <c r="A870" s="25"/>
     </row>
     <row r="871">
-      <c r="A871" s="27"/>
+      <c r="A871" s="25"/>
     </row>
     <row r="872">
-      <c r="A872" s="27"/>
+      <c r="A872" s="25"/>
     </row>
     <row r="873">
-      <c r="A873" s="27"/>
+      <c r="A873" s="25"/>
     </row>
     <row r="874">
-      <c r="A874" s="27"/>
+      <c r="A874" s="25"/>
     </row>
     <row r="875">
-      <c r="A875" s="27"/>
+      <c r="A875" s="25"/>
     </row>
     <row r="876">
-      <c r="A876" s="27"/>
+      <c r="A876" s="25"/>
     </row>
     <row r="877">
-      <c r="A877" s="27"/>
+      <c r="A877" s="25"/>
     </row>
     <row r="878">
-      <c r="A878" s="27"/>
+      <c r="A878" s="25"/>
     </row>
     <row r="879">
-      <c r="A879" s="27"/>
+      <c r="A879" s="25"/>
     </row>
     <row r="880">
-      <c r="A880" s="27"/>
+      <c r="A880" s="25"/>
     </row>
     <row r="881">
-      <c r="A881" s="27"/>
+      <c r="A881" s="25"/>
     </row>
     <row r="882">
-      <c r="A882" s="27"/>
+      <c r="A882" s="25"/>
     </row>
     <row r="883">
-      <c r="A883" s="27"/>
+      <c r="A883" s="25"/>
     </row>
     <row r="884">
-      <c r="A884" s="27"/>
+      <c r="A884" s="25"/>
     </row>
     <row r="885">
-      <c r="A885" s="27"/>
+      <c r="A885" s="25"/>
     </row>
     <row r="886">
-      <c r="A886" s="27"/>
+      <c r="A886" s="25"/>
     </row>
     <row r="887">
-      <c r="A887" s="27"/>
+      <c r="A887" s="25"/>
     </row>
     <row r="888">
-      <c r="A888" s="27"/>
+      <c r="A888" s="25"/>
     </row>
     <row r="889">
-      <c r="A889" s="27"/>
+      <c r="A889" s="25"/>
     </row>
     <row r="890">
-      <c r="A890" s="27"/>
+      <c r="A890" s="25"/>
     </row>
     <row r="891">
-      <c r="A891" s="27"/>
+      <c r="A891" s="25"/>
     </row>
     <row r="892">
-      <c r="A892" s="27"/>
+      <c r="A892" s="25"/>
     </row>
     <row r="893">
-      <c r="A893" s="27"/>
+      <c r="A893" s="25"/>
     </row>
     <row r="894">
-      <c r="A894" s="27"/>
+      <c r="A894" s="25"/>
     </row>
     <row r="895">
-      <c r="A895" s="27"/>
+      <c r="A895" s="25"/>
     </row>
     <row r="896">
-      <c r="A896" s="27"/>
+      <c r="A896" s="25"/>
     </row>
     <row r="897">
-      <c r="A897" s="27"/>
+      <c r="A897" s="25"/>
     </row>
     <row r="898">
-      <c r="A898" s="27"/>
+      <c r="A898" s="25"/>
     </row>
     <row r="899">
-      <c r="A899" s="27"/>
+      <c r="A899" s="25"/>
     </row>
     <row r="900">
-      <c r="A900" s="27"/>
+      <c r="A900" s="25"/>
     </row>
     <row r="901">
-      <c r="A901" s="27"/>
+      <c r="A901" s="25"/>
     </row>
     <row r="902">
-      <c r="A902" s="27"/>
+      <c r="A902" s="25"/>
     </row>
     <row r="903">
-      <c r="A903" s="27"/>
+      <c r="A903" s="25"/>
     </row>
     <row r="904">
-      <c r="A904" s="27"/>
+      <c r="A904" s="25"/>
     </row>
     <row r="905">
-      <c r="A905" s="27"/>
+      <c r="A905" s="25"/>
     </row>
     <row r="906">
-      <c r="A906" s="27"/>
+      <c r="A906" s="25"/>
     </row>
     <row r="907">
-      <c r="A907" s="27"/>
+      <c r="A907" s="25"/>
     </row>
     <row r="908">
-      <c r="A908" s="27"/>
+      <c r="A908" s="25"/>
     </row>
     <row r="909">
-      <c r="A909" s="27"/>
+      <c r="A909" s="25"/>
     </row>
     <row r="910">
-      <c r="A910" s="27"/>
+      <c r="A910" s="25"/>
     </row>
     <row r="911">
-      <c r="A911" s="27"/>
+      <c r="A911" s="25"/>
     </row>
     <row r="912">
-      <c r="A912" s="27"/>
+      <c r="A912" s="25"/>
     </row>
     <row r="913">
-      <c r="A913" s="27"/>
+      <c r="A913" s="25"/>
     </row>
     <row r="914">
-      <c r="A914" s="27"/>
+      <c r="A914" s="25"/>
     </row>
     <row r="915">
-      <c r="A915" s="27"/>
+      <c r="A915" s="25"/>
     </row>
     <row r="916">
-      <c r="A916" s="27"/>
+      <c r="A916" s="25"/>
     </row>
     <row r="917">
-      <c r="A917" s="27"/>
+      <c r="A917" s="25"/>
     </row>
     <row r="918">
-      <c r="A918" s="27"/>
+      <c r="A918" s="25"/>
     </row>
     <row r="919">
-      <c r="A919" s="27"/>
+      <c r="A919" s="25"/>
     </row>
     <row r="920">
-      <c r="A920" s="27"/>
+      <c r="A920" s="25"/>
     </row>
     <row r="921">
-      <c r="A921" s="27"/>
+      <c r="A921" s="25"/>
     </row>
     <row r="922">
-      <c r="A922" s="27"/>
+      <c r="A922" s="25"/>
     </row>
     <row r="923">
-      <c r="A923" s="27"/>
+      <c r="A923" s="25"/>
     </row>
     <row r="924">
-      <c r="A924" s="27"/>
+      <c r="A924" s="25"/>
     </row>
     <row r="925">
-      <c r="A925" s="27"/>
+      <c r="A925" s="25"/>
     </row>
     <row r="926">
-      <c r="A926" s="27"/>
+      <c r="A926" s="25"/>
     </row>
     <row r="927">
-      <c r="A927" s="27"/>
+      <c r="A927" s="25"/>
     </row>
     <row r="928">
-      <c r="A928" s="27"/>
+      <c r="A928" s="25"/>
     </row>
     <row r="929">
-      <c r="A929" s="27"/>
+      <c r="A929" s="25"/>
     </row>
     <row r="930">
-      <c r="A930" s="27"/>
+      <c r="A930" s="25"/>
     </row>
     <row r="931">
-      <c r="A931" s="27"/>
+      <c r="A931" s="25"/>
     </row>
     <row r="932">
-      <c r="A932" s="27"/>
+      <c r="A932" s="25"/>
     </row>
     <row r="933">
-      <c r="A933" s="27"/>
+      <c r="A933" s="25"/>
     </row>
     <row r="934">
-      <c r="A934" s="27"/>
+      <c r="A934" s="25"/>
     </row>
     <row r="935">
-      <c r="A935" s="27"/>
+      <c r="A935" s="25"/>
     </row>
     <row r="936">
-      <c r="A936" s="27"/>
+      <c r="A936" s="25"/>
     </row>
     <row r="937">
-      <c r="A937" s="27"/>
+      <c r="A937" s="25"/>
     </row>
     <row r="938">
-      <c r="A938" s="27"/>
+      <c r="A938" s="25"/>
     </row>
     <row r="939">
-      <c r="A939" s="27"/>
+      <c r="A939" s="25"/>
     </row>
     <row r="940">
-      <c r="A940" s="27"/>
+      <c r="A940" s="25"/>
     </row>
     <row r="941">
-      <c r="A941" s="27"/>
+      <c r="A941" s="25"/>
     </row>
     <row r="942">
-      <c r="A942" s="27"/>
+      <c r="A942" s="25"/>
     </row>
     <row r="943">
-      <c r="A943" s="27"/>
+      <c r="A943" s="25"/>
     </row>
     <row r="944">
-      <c r="A944" s="27"/>
+      <c r="A944" s="25"/>
     </row>
     <row r="945">
-      <c r="A945" s="27"/>
+      <c r="A945" s="25"/>
     </row>
     <row r="946">
-      <c r="A946" s="27"/>
+      <c r="A946" s="25"/>
     </row>
     <row r="947">
-      <c r="A947" s="27"/>
+      <c r="A947" s="25"/>
     </row>
     <row r="948">
-      <c r="A948" s="27"/>
+      <c r="A948" s="25"/>
     </row>
     <row r="949">
-      <c r="A949" s="27"/>
+      <c r="A949" s="25"/>
     </row>
     <row r="950">
-      <c r="A950" s="27"/>
+      <c r="A950" s="25"/>
     </row>
     <row r="951">
-      <c r="A951" s="27"/>
+      <c r="A951" s="25"/>
     </row>
     <row r="952">
-      <c r="A952" s="27"/>
+      <c r="A952" s="25"/>
     </row>
     <row r="953">
-      <c r="A953" s="27"/>
+      <c r="A953" s="25"/>
     </row>
     <row r="954">
-      <c r="A954" s="27"/>
+      <c r="A954" s="25"/>
     </row>
     <row r="955">
-      <c r="A955" s="27"/>
+      <c r="A955" s="25"/>
     </row>
     <row r="956">
-      <c r="A956" s="27"/>
+      <c r="A956" s="25"/>
     </row>
     <row r="957">
-      <c r="A957" s="27"/>
+      <c r="A957" s="25"/>
     </row>
     <row r="958">
-      <c r="A958" s="27"/>
+      <c r="A958" s="25"/>
     </row>
     <row r="959">
-      <c r="A959" s="27"/>
+      <c r="A959" s="25"/>
     </row>
     <row r="960">
-      <c r="A960" s="27"/>
+      <c r="A960" s="25"/>
     </row>
     <row r="961">
-      <c r="A961" s="27"/>
+      <c r="A961" s="25"/>
     </row>
     <row r="962">
-      <c r="A962" s="27"/>
+      <c r="A962" s="25"/>
     </row>
     <row r="963">
-      <c r="A963" s="27"/>
+      <c r="A963" s="25"/>
     </row>
     <row r="964">
-      <c r="A964" s="27"/>
+      <c r="A964" s="25"/>
     </row>
     <row r="965">
-      <c r="A965" s="27"/>
+      <c r="A965" s="25"/>
     </row>
     <row r="966">
-      <c r="A966" s="27"/>
+      <c r="A966" s="25"/>
     </row>
     <row r="967">
-      <c r="A967" s="27"/>
+      <c r="A967" s="25"/>
     </row>
     <row r="968">
-      <c r="A968" s="27"/>
+      <c r="A968" s="25"/>
     </row>
     <row r="969">
-      <c r="A969" s="27"/>
+      <c r="A969" s="25"/>
     </row>
     <row r="970">
-      <c r="A970" s="27"/>
+      <c r="A970" s="25"/>
     </row>
     <row r="971">
-      <c r="A971" s="27"/>
+      <c r="A971" s="25"/>
     </row>
     <row r="972">
-      <c r="A972" s="27"/>
+      <c r="A972" s="25"/>
     </row>
     <row r="973">
-      <c r="A973" s="27"/>
+      <c r="A973" s="25"/>
     </row>
     <row r="974">
-      <c r="A974" s="27"/>
+      <c r="A974" s="25"/>
     </row>
     <row r="975">
-      <c r="A975" s="27"/>
+      <c r="A975" s="25"/>
     </row>
     <row r="976">
-      <c r="A976" s="27"/>
+      <c r="A976" s="25"/>
     </row>
     <row r="977">
-      <c r="A977" s="27"/>
+      <c r="A977" s="25"/>
     </row>
     <row r="978">
-      <c r="A978" s="27"/>
+      <c r="A978" s="25"/>
     </row>
     <row r="979">
-      <c r="A979" s="27"/>
+      <c r="A979" s="25"/>
     </row>
     <row r="980">
-      <c r="A980" s="27"/>
+      <c r="A980" s="25"/>
     </row>
     <row r="981">
-      <c r="A981" s="27"/>
+      <c r="A981" s="25"/>
     </row>
     <row r="982">
-      <c r="A982" s="27"/>
+      <c r="A982" s="25"/>
     </row>
     <row r="983">
-      <c r="A983" s="27"/>
+      <c r="A983" s="25"/>
     </row>
     <row r="984">
-      <c r="A984" s="27"/>
+      <c r="A984" s="25"/>
     </row>
     <row r="985">
-      <c r="A985" s="27"/>
+      <c r="A985" s="25"/>
     </row>
     <row r="986">
-      <c r="A986" s="27"/>
+      <c r="A986" s="25"/>
     </row>
     <row r="987">
-      <c r="A987" s="27"/>
+      <c r="A987" s="25"/>
     </row>
     <row r="988">
-      <c r="A988" s="27"/>
+      <c r="A988" s="25"/>
     </row>
     <row r="989">
-      <c r="A989" s="27"/>
+      <c r="A989" s="25"/>
     </row>
     <row r="990">
-      <c r="A990" s="27"/>
+      <c r="A990" s="25"/>
     </row>
     <row r="991">
-      <c r="A991" s="27"/>
+      <c r="A991" s="25"/>
     </row>
     <row r="992">
-      <c r="A992" s="27"/>
+      <c r="A992" s="25"/>
     </row>
     <row r="993">
-      <c r="A993" s="27"/>
+      <c r="A993" s="25"/>
     </row>
     <row r="994">
-      <c r="A994" s="27"/>
+      <c r="A994" s="25"/>
     </row>
     <row r="995">
-      <c r="A995" s="27"/>
+      <c r="A995" s="25"/>
     </row>
     <row r="996">
-      <c r="A996" s="27"/>
+      <c r="A996" s="25"/>
     </row>
     <row r="997">
-      <c r="A997" s="27"/>
+      <c r="A997" s="25"/>
     </row>
     <row r="998">
-      <c r="A998" s="27"/>
+      <c r="A998" s="25"/>
     </row>
     <row r="999">
-      <c r="A999" s="27"/>
+      <c r="A999" s="25"/>
     </row>
     <row r="1000">
-      <c r="A1000" s="27"/>
+      <c r="A1000" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>